<commit_message>
Costs per task Update
</commit_message>
<xml_diff>
--- a/Deliverable 2/Deliverable2/Costs task 8_v2.xlsx
+++ b/Deliverable 2/Deliverable2/Costs task 8_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Santi/Documents/GitHub/projectsGroup3/Deliverable 2/Deliverable2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82998650-D4CA-F749-9E3D-63BEAD3B14E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9810226F-7CFE-5649-91CF-E03D20616AA5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,7 +648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,7 +679,6 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1398,16 +1397,16 @@
   <dimension ref="A1:AL65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC67" sqref="AC67"/>
+      <selection pane="bottomRight" activeCell="AG60" sqref="AG60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="3.83203125" customWidth="1"/>
+    <col min="3" max="5" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -1421,9 +1420,7 @@
     <col min="31" max="32" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1580,21 +1577,25 @@
         <f>AF2*C2*DATOS!$B$3+'COST PER TASK'!AF2*'COST PER TASK'!D2*DATOS!$B$4+'COST PER TASK'!AF2*'COST PER TASK'!E2*DATOS!$B$5</f>
         <v>3280</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AH2" s="4">
         <f>F2*AE2*DATOS!$D$6+'COST PER TASK'!G2*'COST PER TASK'!AE2*DATOS!$D$7+'COST PER TASK'!H2*'COST PER TASK'!AE2*DATOS!$D$8+'COST PER TASK'!I2*'COST PER TASK'!AE2*DATOS!$D$9+'COST PER TASK'!J2*'COST PER TASK'!AE2*DATOS!$D$10+'COST PER TASK'!K2*'COST PER TASK'!AE2*DATOS!$D$11+'COST PER TASK'!L2*'COST PER TASK'!AE2*DATOS!$D$12+'COST PER TASK'!M2*'COST PER TASK'!AE2*DATOS!$D$13+'COST PER TASK'!N2*'COST PER TASK'!AE2*DATOS!$D$14+'COST PER TASK'!O2*'COST PER TASK'!AE2*DATOS!$D$15</f>
         <v>70.77988825667596</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AI2" s="4">
         <f>'COST PER TASK'!P2*'COST PER TASK'!AE2*DATOS!$D$16+'COST PER TASK'!Q2*'COST PER TASK'!AE2*DATOS!$D$17+'COST PER TASK'!R2*'COST PER TASK'!AE2*DATOS!$D$18+'COST PER TASK'!S2*'COST PER TASK'!AE2*DATOS!$D$19+'COST PER TASK'!T2*'COST PER TASK'!AE2*DATOS!$D$20+'COST PER TASK'!U2*'COST PER TASK'!AE2*DATOS!$D$21+'COST PER TASK'!V2*'COST PER TASK'!AE2*DATOS!$D$22</f>
         <v>0</v>
+      </c>
+      <c r="AJ2" s="4">
+        <f>'COST PER TASK'!W2*'COST PER TASK'!AE2*DATOS!$B$23+'COST PER TASK'!X2*'COST PER TASK'!AE2*DATOS!$B$24+'COST PER TASK'!Y2*'COST PER TASK'!AE2*DATOS!$B$25+'COST PER TASK'!Z2*'COST PER TASK'!AE2*DATOS!$B$26+'COST PER TASK'!AA2*'COST PER TASK'!AE2*DATOS!$B$27+'COST PER TASK'!AB2*'COST PER TASK'!AE2*DATOS!$B$28+'COST PER TASK'!AC2*'COST PER TASK'!AE2*DATOS!$B$29</f>
+        <v>800</v>
       </c>
       <c r="AK2" s="8">
         <f>AG2+AH2+AI2+AJ2</f>
-        <v>3350.7798882566758</v>
+        <v>4150.7798882566758</v>
       </c>
       <c r="AL2" s="8">
         <f>AK2/AD2</f>
-        <v>167.5389944128338</v>
+        <v>207.5389944128338</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
@@ -1631,21 +1632,25 @@
         <f>AF3*C3*DATOS!$B$3+'COST PER TASK'!AF3*'COST PER TASK'!D3*DATOS!$B$4+'COST PER TASK'!AF3*'COST PER TASK'!E3*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AH3" s="4">
         <f>F3*AE3*DATOS!$D$6+'COST PER TASK'!G3*'COST PER TASK'!AE3*DATOS!$D$7+'COST PER TASK'!H3*'COST PER TASK'!AE3*DATOS!$D$8+'COST PER TASK'!I3*'COST PER TASK'!AE3*DATOS!$D$9+'COST PER TASK'!J3*'COST PER TASK'!AE3*DATOS!$D$10+'COST PER TASK'!K3*'COST PER TASK'!AE3*DATOS!$D$11+'COST PER TASK'!L3*'COST PER TASK'!AE3*DATOS!$D$12+'COST PER TASK'!M3*'COST PER TASK'!AE3*DATOS!$D$13+'COST PER TASK'!N3*'COST PER TASK'!AE3*DATOS!$D$14+'COST PER TASK'!O3*'COST PER TASK'!AE3*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AI3" s="4">
         <f>'COST PER TASK'!P3*'COST PER TASK'!AE3*DATOS!$D$16+'COST PER TASK'!Q3*'COST PER TASK'!AE3*DATOS!$D$17+'COST PER TASK'!R3*'COST PER TASK'!AE3*DATOS!$D$18+'COST PER TASK'!S3*'COST PER TASK'!AE3*DATOS!$D$19+'COST PER TASK'!T3*'COST PER TASK'!AE3*DATOS!$D$20+'COST PER TASK'!U3*'COST PER TASK'!AE3*DATOS!$D$21+'COST PER TASK'!V3*'COST PER TASK'!AE3*DATOS!$D$22</f>
         <v>0</v>
+      </c>
+      <c r="AJ3" s="4">
+        <f>'COST PER TASK'!W3*'COST PER TASK'!AE3*DATOS!$B$23+'COST PER TASK'!X3*'COST PER TASK'!AE3*DATOS!$B$24+'COST PER TASK'!Y3*'COST PER TASK'!AE3*DATOS!$B$25+'COST PER TASK'!Z3*'COST PER TASK'!AE3*DATOS!$B$26+'COST PER TASK'!AA3*'COST PER TASK'!AE3*DATOS!$B$27+'COST PER TASK'!AB3*'COST PER TASK'!AE3*DATOS!$B$28+'COST PER TASK'!AC3*'COST PER TASK'!AE3*DATOS!$B$29</f>
+        <v>7040</v>
       </c>
       <c r="AK3" s="8">
         <f t="shared" ref="AK3:AK64" si="1">AG3+AH3+AI3+AJ3</f>
-        <v>144320</v>
+        <v>151360</v>
       </c>
       <c r="AL3" s="8">
         <f t="shared" ref="AL3:AL64" si="2">AK3/AD3</f>
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
@@ -1682,21 +1687,25 @@
         <f>AF4*C4*DATOS!$B$3+'COST PER TASK'!AF4*'COST PER TASK'!D4*DATOS!$B$4+'COST PER TASK'!AF4*'COST PER TASK'!E4*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AH4" s="4">
         <f>F4*AE4*DATOS!$D$6+'COST PER TASK'!G4*'COST PER TASK'!AE4*DATOS!$D$7+'COST PER TASK'!H4*'COST PER TASK'!AE4*DATOS!$D$8+'COST PER TASK'!I4*'COST PER TASK'!AE4*DATOS!$D$9+'COST PER TASK'!J4*'COST PER TASK'!AE4*DATOS!$D$10+'COST PER TASK'!K4*'COST PER TASK'!AE4*DATOS!$D$11+'COST PER TASK'!L4*'COST PER TASK'!AE4*DATOS!$D$12+'COST PER TASK'!M4*'COST PER TASK'!AE4*DATOS!$D$13+'COST PER TASK'!N4*'COST PER TASK'!AE4*DATOS!$D$14+'COST PER TASK'!O4*'COST PER TASK'!AE4*DATOS!$D$15</f>
         <v>4264</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AI4" s="4">
         <f>'COST PER TASK'!P4*'COST PER TASK'!AE4*DATOS!$D$16+'COST PER TASK'!Q4*'COST PER TASK'!AE4*DATOS!$D$17+'COST PER TASK'!R4*'COST PER TASK'!AE4*DATOS!$D$18+'COST PER TASK'!S4*'COST PER TASK'!AE4*DATOS!$D$19+'COST PER TASK'!T4*'COST PER TASK'!AE4*DATOS!$D$20+'COST PER TASK'!U4*'COST PER TASK'!AE4*DATOS!$D$21+'COST PER TASK'!V4*'COST PER TASK'!AE4*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ4" s="4">
+        <f>'COST PER TASK'!W4*'COST PER TASK'!AE4*DATOS!$B$23+'COST PER TASK'!X4*'COST PER TASK'!AE4*DATOS!$B$24+'COST PER TASK'!Y4*'COST PER TASK'!AE4*DATOS!$B$25+'COST PER TASK'!Z4*'COST PER TASK'!AE4*DATOS!$B$26+'COST PER TASK'!AA4*'COST PER TASK'!AE4*DATOS!$B$27+'COST PER TASK'!AB4*'COST PER TASK'!AE4*DATOS!$B$28+'COST PER TASK'!AC4*'COST PER TASK'!AE4*DATOS!$B$29</f>
+        <v>7040</v>
+      </c>
       <c r="AK4" s="8">
         <f t="shared" si="1"/>
-        <v>148584</v>
+        <v>155624</v>
       </c>
       <c r="AL4" s="8">
         <f t="shared" si="2"/>
-        <v>168.84545454545454</v>
+        <v>176.84545454545454</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
@@ -1739,21 +1748,25 @@
         <f>AF5*C5*DATOS!$B$3+'COST PER TASK'!AF5*'COST PER TASK'!D5*DATOS!$B$4+'COST PER TASK'!AF5*'COST PER TASK'!E5*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH5" s="3">
+      <c r="AH5" s="4">
         <f>F5*AE5*DATOS!$D$6+'COST PER TASK'!G5*'COST PER TASK'!AE5*DATOS!$D$7+'COST PER TASK'!H5*'COST PER TASK'!AE5*DATOS!$D$8+'COST PER TASK'!I5*'COST PER TASK'!AE5*DATOS!$D$9+'COST PER TASK'!J5*'COST PER TASK'!AE5*DATOS!$D$10+'COST PER TASK'!K5*'COST PER TASK'!AE5*DATOS!$D$11+'COST PER TASK'!L5*'COST PER TASK'!AE5*DATOS!$D$12+'COST PER TASK'!M5*'COST PER TASK'!AE5*DATOS!$D$13+'COST PER TASK'!N5*'COST PER TASK'!AE5*DATOS!$D$14+'COST PER TASK'!O5*'COST PER TASK'!AE5*DATOS!$D$15</f>
         <v>3114.3150832937426</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="AI5" s="4">
         <f>'COST PER TASK'!P5*'COST PER TASK'!AE5*DATOS!$D$16+'COST PER TASK'!Q5*'COST PER TASK'!AE5*DATOS!$D$17+'COST PER TASK'!R5*'COST PER TASK'!AE5*DATOS!$D$18+'COST PER TASK'!S5*'COST PER TASK'!AE5*DATOS!$D$19+'COST PER TASK'!T5*'COST PER TASK'!AE5*DATOS!$D$20+'COST PER TASK'!U5*'COST PER TASK'!AE5*DATOS!$D$21+'COST PER TASK'!V5*'COST PER TASK'!AE5*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ5" s="4">
+        <f>'COST PER TASK'!W5*'COST PER TASK'!AE5*DATOS!$B$23+'COST PER TASK'!X5*'COST PER TASK'!AE5*DATOS!$B$24+'COST PER TASK'!Y5*'COST PER TASK'!AE5*DATOS!$B$25+'COST PER TASK'!Z5*'COST PER TASK'!AE5*DATOS!$B$26+'COST PER TASK'!AA5*'COST PER TASK'!AE5*DATOS!$B$27+'COST PER TASK'!AB5*'COST PER TASK'!AE5*DATOS!$B$28+'COST PER TASK'!AC5*'COST PER TASK'!AE5*DATOS!$B$29</f>
+        <v>49280</v>
+      </c>
       <c r="AK5" s="8">
         <f t="shared" si="1"/>
-        <v>147434.31508329374</v>
+        <v>196714.31508329374</v>
       </c>
       <c r="AL5" s="8">
         <f t="shared" si="2"/>
-        <v>167.5389944128338</v>
+        <v>223.5389944128338</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
@@ -1784,21 +1797,25 @@
         <f>AF6*C6*DATOS!$B$3+'COST PER TASK'!AF6*'COST PER TASK'!D6*DATOS!$B$4+'COST PER TASK'!AF6*'COST PER TASK'!E6*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH6" s="3">
+      <c r="AH6" s="4">
         <f>F6*AE6*DATOS!$D$6+'COST PER TASK'!G6*'COST PER TASK'!AE6*DATOS!$D$7+'COST PER TASK'!H6*'COST PER TASK'!AE6*DATOS!$D$8+'COST PER TASK'!I6*'COST PER TASK'!AE6*DATOS!$D$9+'COST PER TASK'!J6*'COST PER TASK'!AE6*DATOS!$D$10+'COST PER TASK'!K6*'COST PER TASK'!AE6*DATOS!$D$11+'COST PER TASK'!L6*'COST PER TASK'!AE6*DATOS!$D$12+'COST PER TASK'!M6*'COST PER TASK'!AE6*DATOS!$D$13+'COST PER TASK'!N6*'COST PER TASK'!AE6*DATOS!$D$14+'COST PER TASK'!O6*'COST PER TASK'!AE6*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AI6" s="4">
         <f>'COST PER TASK'!P6*'COST PER TASK'!AE6*DATOS!$D$16+'COST PER TASK'!Q6*'COST PER TASK'!AE6*DATOS!$D$17+'COST PER TASK'!R6*'COST PER TASK'!AE6*DATOS!$D$18+'COST PER TASK'!S6*'COST PER TASK'!AE6*DATOS!$D$19+'COST PER TASK'!T6*'COST PER TASK'!AE6*DATOS!$D$20+'COST PER TASK'!U6*'COST PER TASK'!AE6*DATOS!$D$21+'COST PER TASK'!V6*'COST PER TASK'!AE6*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ6" s="4">
+        <f>'COST PER TASK'!W6*'COST PER TASK'!AE6*DATOS!$B$23+'COST PER TASK'!X6*'COST PER TASK'!AE6*DATOS!$B$24+'COST PER TASK'!Y6*'COST PER TASK'!AE6*DATOS!$B$25+'COST PER TASK'!Z6*'COST PER TASK'!AE6*DATOS!$B$26+'COST PER TASK'!AA6*'COST PER TASK'!AE6*DATOS!$B$27+'COST PER TASK'!AB6*'COST PER TASK'!AE6*DATOS!$B$28+'COST PER TASK'!AC6*'COST PER TASK'!AE6*DATOS!$B$29</f>
+        <v>35200</v>
+      </c>
       <c r="AK6" s="8">
         <f t="shared" si="1"/>
-        <v>144320</v>
+        <v>179520</v>
       </c>
       <c r="AL6" s="8">
         <f t="shared" si="2"/>
-        <v>164</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
@@ -1829,21 +1846,25 @@
         <f>AF7*C7*DATOS!$B$3+'COST PER TASK'!AF7*'COST PER TASK'!D7*DATOS!$B$4+'COST PER TASK'!AF7*'COST PER TASK'!E7*DATOS!$B$5</f>
         <v>4920</v>
       </c>
-      <c r="AH7" s="3">
+      <c r="AH7" s="4">
         <f>F7*AE7*DATOS!$D$6+'COST PER TASK'!G7*'COST PER TASK'!AE7*DATOS!$D$7+'COST PER TASK'!H7*'COST PER TASK'!AE7*DATOS!$D$8+'COST PER TASK'!I7*'COST PER TASK'!AE7*DATOS!$D$9+'COST PER TASK'!J7*'COST PER TASK'!AE7*DATOS!$D$10+'COST PER TASK'!K7*'COST PER TASK'!AE7*DATOS!$D$11+'COST PER TASK'!L7*'COST PER TASK'!AE7*DATOS!$D$12+'COST PER TASK'!M7*'COST PER TASK'!AE7*DATOS!$D$13+'COST PER TASK'!N7*'COST PER TASK'!AE7*DATOS!$D$14+'COST PER TASK'!O7*'COST PER TASK'!AE7*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI7" s="3">
+      <c r="AI7" s="4">
         <f>'COST PER TASK'!P7*'COST PER TASK'!AE7*DATOS!$D$16+'COST PER TASK'!Q7*'COST PER TASK'!AE7*DATOS!$D$17+'COST PER TASK'!R7*'COST PER TASK'!AE7*DATOS!$D$18+'COST PER TASK'!S7*'COST PER TASK'!AE7*DATOS!$D$19+'COST PER TASK'!T7*'COST PER TASK'!AE7*DATOS!$D$20+'COST PER TASK'!U7*'COST PER TASK'!AE7*DATOS!$D$21+'COST PER TASK'!V7*'COST PER TASK'!AE7*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ7" s="4">
+        <f>'COST PER TASK'!W7*'COST PER TASK'!AE7*DATOS!$B$23+'COST PER TASK'!X7*'COST PER TASK'!AE7*DATOS!$B$24+'COST PER TASK'!Y7*'COST PER TASK'!AE7*DATOS!$B$25+'COST PER TASK'!Z7*'COST PER TASK'!AE7*DATOS!$B$26+'COST PER TASK'!AA7*'COST PER TASK'!AE7*DATOS!$B$27+'COST PER TASK'!AB7*'COST PER TASK'!AE7*DATOS!$B$28+'COST PER TASK'!AC7*'COST PER TASK'!AE7*DATOS!$B$29</f>
+        <v>1200</v>
+      </c>
       <c r="AK7" s="8">
         <f t="shared" si="1"/>
-        <v>4920</v>
+        <v>6120</v>
       </c>
       <c r="AL7" s="8">
         <f t="shared" si="2"/>
-        <v>164</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
@@ -1874,21 +1895,25 @@
         <f>AF8*C8*DATOS!$B$3+'COST PER TASK'!AF8*'COST PER TASK'!D8*DATOS!$B$4+'COST PER TASK'!AF8*'COST PER TASK'!E8*DATOS!$B$5</f>
         <v>136120</v>
       </c>
-      <c r="AH8" s="3">
+      <c r="AH8" s="4">
         <f>F8*AE8*DATOS!$D$6+'COST PER TASK'!G8*'COST PER TASK'!AE8*DATOS!$D$7+'COST PER TASK'!H8*'COST PER TASK'!AE8*DATOS!$D$8+'COST PER TASK'!I8*'COST PER TASK'!AE8*DATOS!$D$9+'COST PER TASK'!J8*'COST PER TASK'!AE8*DATOS!$D$10+'COST PER TASK'!K8*'COST PER TASK'!AE8*DATOS!$D$11+'COST PER TASK'!L8*'COST PER TASK'!AE8*DATOS!$D$12+'COST PER TASK'!M8*'COST PER TASK'!AE8*DATOS!$D$13+'COST PER TASK'!N8*'COST PER TASK'!AE8*DATOS!$D$14+'COST PER TASK'!O8*'COST PER TASK'!AE8*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="3">
+      <c r="AI8" s="4">
         <f>'COST PER TASK'!P8*'COST PER TASK'!AE8*DATOS!$D$16+'COST PER TASK'!Q8*'COST PER TASK'!AE8*DATOS!$D$17+'COST PER TASK'!R8*'COST PER TASK'!AE8*DATOS!$D$18+'COST PER TASK'!S8*'COST PER TASK'!AE8*DATOS!$D$19+'COST PER TASK'!T8*'COST PER TASK'!AE8*DATOS!$D$20+'COST PER TASK'!U8*'COST PER TASK'!AE8*DATOS!$D$21+'COST PER TASK'!V8*'COST PER TASK'!AE8*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ8" s="4">
+        <f>'COST PER TASK'!W8*'COST PER TASK'!AE8*DATOS!$B$23+'COST PER TASK'!X8*'COST PER TASK'!AE8*DATOS!$B$24+'COST PER TASK'!Y8*'COST PER TASK'!AE8*DATOS!$B$25+'COST PER TASK'!Z8*'COST PER TASK'!AE8*DATOS!$B$26+'COST PER TASK'!AA8*'COST PER TASK'!AE8*DATOS!$B$27+'COST PER TASK'!AB8*'COST PER TASK'!AE8*DATOS!$B$28+'COST PER TASK'!AC8*'COST PER TASK'!AE8*DATOS!$B$29</f>
+        <v>33200</v>
+      </c>
       <c r="AK8" s="8">
         <f t="shared" si="1"/>
-        <v>136120</v>
+        <v>169320</v>
       </c>
       <c r="AL8" s="8">
         <f>AK8/AD8</f>
-        <v>164</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
@@ -1928,21 +1953,25 @@
         <f>AF9*C9*DATOS!$B$3+'COST PER TASK'!AF9*'COST PER TASK'!D9*DATOS!$B$4+'COST PER TASK'!AF9*'COST PER TASK'!E9*DATOS!$B$5</f>
         <v>328</v>
       </c>
-      <c r="AH9" s="3">
+      <c r="AH9" s="4">
         <f>F9*AE9*DATOS!$D$6+'COST PER TASK'!G9*'COST PER TASK'!AE9*DATOS!$D$7+'COST PER TASK'!H9*'COST PER TASK'!AE9*DATOS!$D$8+'COST PER TASK'!I9*'COST PER TASK'!AE9*DATOS!$D$9+'COST PER TASK'!J9*'COST PER TASK'!AE9*DATOS!$D$10+'COST PER TASK'!K9*'COST PER TASK'!AE9*DATOS!$D$11+'COST PER TASK'!L9*'COST PER TASK'!AE9*DATOS!$D$12+'COST PER TASK'!M9*'COST PER TASK'!AE9*DATOS!$D$13+'COST PER TASK'!N9*'COST PER TASK'!AE9*DATOS!$D$14+'COST PER TASK'!O9*'COST PER TASK'!AE9*DATOS!$D$15</f>
         <v>48.077988825667596</v>
       </c>
-      <c r="AI9" s="3">
+      <c r="AI9" s="4">
         <f>'COST PER TASK'!P9*'COST PER TASK'!AE9*DATOS!$D$16+'COST PER TASK'!Q9*'COST PER TASK'!AE9*DATOS!$D$17+'COST PER TASK'!R9*'COST PER TASK'!AE9*DATOS!$D$18+'COST PER TASK'!S9*'COST PER TASK'!AE9*DATOS!$D$19+'COST PER TASK'!T9*'COST PER TASK'!AE9*DATOS!$D$20+'COST PER TASK'!U9*'COST PER TASK'!AE9*DATOS!$D$21+'COST PER TASK'!V9*'COST PER TASK'!AE9*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ9" s="4">
+        <f>'COST PER TASK'!W9*'COST PER TASK'!AE9*DATOS!$B$23+'COST PER TASK'!X9*'COST PER TASK'!AE9*DATOS!$B$24+'COST PER TASK'!Y9*'COST PER TASK'!AE9*DATOS!$B$25+'COST PER TASK'!Z9*'COST PER TASK'!AE9*DATOS!$B$26+'COST PER TASK'!AA9*'COST PER TASK'!AE9*DATOS!$B$27+'COST PER TASK'!AB9*'COST PER TASK'!AE9*DATOS!$B$28+'COST PER TASK'!AC9*'COST PER TASK'!AE9*DATOS!$B$29</f>
+        <v>80</v>
+      </c>
       <c r="AK9" s="8">
         <f t="shared" si="1"/>
-        <v>376.0779888256676</v>
+        <v>456.0779888256676</v>
       </c>
       <c r="AL9" s="8">
         <f t="shared" si="2"/>
-        <v>188.0389944128338</v>
+        <v>228.0389944128338</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
@@ -1982,21 +2011,25 @@
         <f>AF10*C10*DATOS!$B$3+'COST PER TASK'!AF10*'COST PER TASK'!D10*DATOS!$B$4+'COST PER TASK'!AF10*'COST PER TASK'!E10*DATOS!$B$5</f>
         <v>328</v>
       </c>
-      <c r="AH10" s="3">
+      <c r="AH10" s="4">
         <f>F10*AE10*DATOS!$D$6+'COST PER TASK'!G10*'COST PER TASK'!AE10*DATOS!$D$7+'COST PER TASK'!H10*'COST PER TASK'!AE10*DATOS!$D$8+'COST PER TASK'!I10*'COST PER TASK'!AE10*DATOS!$D$9+'COST PER TASK'!J10*'COST PER TASK'!AE10*DATOS!$D$10+'COST PER TASK'!K10*'COST PER TASK'!AE10*DATOS!$D$11+'COST PER TASK'!L10*'COST PER TASK'!AE10*DATOS!$D$12+'COST PER TASK'!M10*'COST PER TASK'!AE10*DATOS!$D$13+'COST PER TASK'!N10*'COST PER TASK'!AE10*DATOS!$D$14+'COST PER TASK'!O10*'COST PER TASK'!AE10*DATOS!$D$15</f>
         <v>48.077988825667596</v>
       </c>
-      <c r="AI10" s="3">
+      <c r="AI10" s="4">
         <f>'COST PER TASK'!P10*'COST PER TASK'!AE10*DATOS!$D$16+'COST PER TASK'!Q10*'COST PER TASK'!AE10*DATOS!$D$17+'COST PER TASK'!R10*'COST PER TASK'!AE10*DATOS!$D$18+'COST PER TASK'!S10*'COST PER TASK'!AE10*DATOS!$D$19+'COST PER TASK'!T10*'COST PER TASK'!AE10*DATOS!$D$20+'COST PER TASK'!U10*'COST PER TASK'!AE10*DATOS!$D$21+'COST PER TASK'!V10*'COST PER TASK'!AE10*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ10" s="4">
+        <f>'COST PER TASK'!W10*'COST PER TASK'!AE10*DATOS!$B$23+'COST PER TASK'!X10*'COST PER TASK'!AE10*DATOS!$B$24+'COST PER TASK'!Y10*'COST PER TASK'!AE10*DATOS!$B$25+'COST PER TASK'!Z10*'COST PER TASK'!AE10*DATOS!$B$26+'COST PER TASK'!AA10*'COST PER TASK'!AE10*DATOS!$B$27+'COST PER TASK'!AB10*'COST PER TASK'!AE10*DATOS!$B$28+'COST PER TASK'!AC10*'COST PER TASK'!AE10*DATOS!$B$29</f>
+        <v>80</v>
+      </c>
       <c r="AK10" s="8">
         <f t="shared" si="1"/>
-        <v>376.0779888256676</v>
+        <v>456.0779888256676</v>
       </c>
       <c r="AL10" s="8">
         <f t="shared" si="2"/>
-        <v>188.0389944128338</v>
+        <v>228.0389944128338</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.2">
@@ -2036,21 +2069,25 @@
         <f>AF11*C11*DATOS!$B$3+'COST PER TASK'!AF11*'COST PER TASK'!D11*DATOS!$B$4+'COST PER TASK'!AF11*'COST PER TASK'!E11*DATOS!$B$5</f>
         <v>492</v>
       </c>
-      <c r="AH11" s="3">
+      <c r="AH11" s="4">
         <f>F11*AE11*DATOS!$D$6+'COST PER TASK'!G11*'COST PER TASK'!AE11*DATOS!$D$7+'COST PER TASK'!H11*'COST PER TASK'!AE11*DATOS!$D$8+'COST PER TASK'!I11*'COST PER TASK'!AE11*DATOS!$D$9+'COST PER TASK'!J11*'COST PER TASK'!AE11*DATOS!$D$10+'COST PER TASK'!K11*'COST PER TASK'!AE11*DATOS!$D$11+'COST PER TASK'!L11*'COST PER TASK'!AE11*DATOS!$D$12+'COST PER TASK'!M11*'COST PER TASK'!AE11*DATOS!$D$13+'COST PER TASK'!N11*'COST PER TASK'!AE11*DATOS!$D$14+'COST PER TASK'!O11*'COST PER TASK'!AE11*DATOS!$D$15</f>
         <v>72.11698323850139</v>
       </c>
-      <c r="AI11" s="3">
+      <c r="AI11" s="4">
         <f>'COST PER TASK'!P11*'COST PER TASK'!AE11*DATOS!$D$16+'COST PER TASK'!Q11*'COST PER TASK'!AE11*DATOS!$D$17+'COST PER TASK'!R11*'COST PER TASK'!AE11*DATOS!$D$18+'COST PER TASK'!S11*'COST PER TASK'!AE11*DATOS!$D$19+'COST PER TASK'!T11*'COST PER TASK'!AE11*DATOS!$D$20+'COST PER TASK'!U11*'COST PER TASK'!AE11*DATOS!$D$21+'COST PER TASK'!V11*'COST PER TASK'!AE11*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ11" s="4">
+        <f>'COST PER TASK'!W11*'COST PER TASK'!AE11*DATOS!$B$23+'COST PER TASK'!X11*'COST PER TASK'!AE11*DATOS!$B$24+'COST PER TASK'!Y11*'COST PER TASK'!AE11*DATOS!$B$25+'COST PER TASK'!Z11*'COST PER TASK'!AE11*DATOS!$B$26+'COST PER TASK'!AA11*'COST PER TASK'!AE11*DATOS!$B$27+'COST PER TASK'!AB11*'COST PER TASK'!AE11*DATOS!$B$28+'COST PER TASK'!AC11*'COST PER TASK'!AE11*DATOS!$B$29</f>
+        <v>120</v>
+      </c>
       <c r="AK11" s="8">
         <f t="shared" si="1"/>
-        <v>564.11698323850135</v>
+        <v>684.11698323850135</v>
       </c>
       <c r="AL11" s="8">
         <f t="shared" si="2"/>
-        <v>188.03899441283377</v>
+        <v>228.03899441283377</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
@@ -2090,21 +2127,25 @@
         <f>AF12*C12*DATOS!$B$3+'COST PER TASK'!AF12*'COST PER TASK'!D12*DATOS!$B$4+'COST PER TASK'!AF12*'COST PER TASK'!E12*DATOS!$B$5</f>
         <v>820</v>
       </c>
-      <c r="AH12" s="3">
+      <c r="AH12" s="4">
         <f>F12*AE12*DATOS!$D$6+'COST PER TASK'!G12*'COST PER TASK'!AE12*DATOS!$D$7+'COST PER TASK'!H12*'COST PER TASK'!AE12*DATOS!$D$8+'COST PER TASK'!I12*'COST PER TASK'!AE12*DATOS!$D$9+'COST PER TASK'!J12*'COST PER TASK'!AE12*DATOS!$D$10+'COST PER TASK'!K12*'COST PER TASK'!AE12*DATOS!$D$11+'COST PER TASK'!L12*'COST PER TASK'!AE12*DATOS!$D$12+'COST PER TASK'!M12*'COST PER TASK'!AE12*DATOS!$D$13+'COST PER TASK'!N12*'COST PER TASK'!AE12*DATOS!$D$14+'COST PER TASK'!O12*'COST PER TASK'!AE12*DATOS!$D$15</f>
         <v>120.19497206416899</v>
       </c>
-      <c r="AI12" s="3">
+      <c r="AI12" s="4">
         <f>'COST PER TASK'!P12*'COST PER TASK'!AE12*DATOS!$D$16+'COST PER TASK'!Q12*'COST PER TASK'!AE12*DATOS!$D$17+'COST PER TASK'!R12*'COST PER TASK'!AE12*DATOS!$D$18+'COST PER TASK'!S12*'COST PER TASK'!AE12*DATOS!$D$19+'COST PER TASK'!T12*'COST PER TASK'!AE12*DATOS!$D$20+'COST PER TASK'!U12*'COST PER TASK'!AE12*DATOS!$D$21+'COST PER TASK'!V12*'COST PER TASK'!AE12*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ12" s="4">
+        <f>'COST PER TASK'!W12*'COST PER TASK'!AE12*DATOS!$B$23+'COST PER TASK'!X12*'COST PER TASK'!AE12*DATOS!$B$24+'COST PER TASK'!Y12*'COST PER TASK'!AE12*DATOS!$B$25+'COST PER TASK'!Z12*'COST PER TASK'!AE12*DATOS!$B$26+'COST PER TASK'!AA12*'COST PER TASK'!AE12*DATOS!$B$27+'COST PER TASK'!AB12*'COST PER TASK'!AE12*DATOS!$B$28+'COST PER TASK'!AC12*'COST PER TASK'!AE12*DATOS!$B$29</f>
+        <v>200</v>
+      </c>
       <c r="AK12" s="8">
         <f t="shared" si="1"/>
-        <v>940.19497206416895</v>
+        <v>1140.194972064169</v>
       </c>
       <c r="AL12" s="8">
         <f t="shared" si="2"/>
-        <v>188.0389944128338</v>
+        <v>228.0389944128338</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">
@@ -2141,21 +2182,25 @@
         <f>AF13*C13*DATOS!$B$3+'COST PER TASK'!AF13*'COST PER TASK'!D13*DATOS!$B$4+'COST PER TASK'!AF13*'COST PER TASK'!E13*DATOS!$B$5</f>
         <v>820</v>
       </c>
-      <c r="AH13" s="3">
+      <c r="AH13" s="4">
         <f>F13*AE13*DATOS!$D$6+'COST PER TASK'!G13*'COST PER TASK'!AE13*DATOS!$D$7+'COST PER TASK'!H13*'COST PER TASK'!AE13*DATOS!$D$8+'COST PER TASK'!I13*'COST PER TASK'!AE13*DATOS!$D$9+'COST PER TASK'!J13*'COST PER TASK'!AE13*DATOS!$D$10+'COST PER TASK'!K13*'COST PER TASK'!AE13*DATOS!$D$11+'COST PER TASK'!L13*'COST PER TASK'!AE13*DATOS!$D$12+'COST PER TASK'!M13*'COST PER TASK'!AE13*DATOS!$D$13+'COST PER TASK'!N13*'COST PER TASK'!AE13*DATOS!$D$14+'COST PER TASK'!O13*'COST PER TASK'!AE13*DATOS!$D$15</f>
         <v>17.69497206416899</v>
       </c>
-      <c r="AI13" s="3">
+      <c r="AI13" s="4">
         <f>'COST PER TASK'!P13*'COST PER TASK'!AE13*DATOS!$D$16+'COST PER TASK'!Q13*'COST PER TASK'!AE13*DATOS!$D$17+'COST PER TASK'!R13*'COST PER TASK'!AE13*DATOS!$D$18+'COST PER TASK'!S13*'COST PER TASK'!AE13*DATOS!$D$19+'COST PER TASK'!T13*'COST PER TASK'!AE13*DATOS!$D$20+'COST PER TASK'!U13*'COST PER TASK'!AE13*DATOS!$D$21+'COST PER TASK'!V13*'COST PER TASK'!AE13*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ13" s="4">
+        <f>'COST PER TASK'!W13*'COST PER TASK'!AE13*DATOS!$B$23+'COST PER TASK'!X13*'COST PER TASK'!AE13*DATOS!$B$24+'COST PER TASK'!Y13*'COST PER TASK'!AE13*DATOS!$B$25+'COST PER TASK'!Z13*'COST PER TASK'!AE13*DATOS!$B$26+'COST PER TASK'!AA13*'COST PER TASK'!AE13*DATOS!$B$27+'COST PER TASK'!AB13*'COST PER TASK'!AE13*DATOS!$B$28+'COST PER TASK'!AC13*'COST PER TASK'!AE13*DATOS!$B$29</f>
+        <v>200</v>
+      </c>
       <c r="AK13" s="8">
         <f t="shared" si="1"/>
-        <v>837.69497206416895</v>
+        <v>1037.694972064169</v>
       </c>
       <c r="AL13" s="8">
         <f t="shared" si="2"/>
-        <v>167.5389944128338</v>
+        <v>207.5389944128338</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.2">
@@ -2186,21 +2231,25 @@
         <f>AF14*C14*DATOS!$B$3+'COST PER TASK'!AF14*'COST PER TASK'!D14*DATOS!$B$4+'COST PER TASK'!AF14*'COST PER TASK'!E14*DATOS!$B$5</f>
         <v>492</v>
       </c>
-      <c r="AH14" s="3">
+      <c r="AH14" s="4">
         <f>F14*AE14*DATOS!$D$6+'COST PER TASK'!G14*'COST PER TASK'!AE14*DATOS!$D$7+'COST PER TASK'!H14*'COST PER TASK'!AE14*DATOS!$D$8+'COST PER TASK'!I14*'COST PER TASK'!AE14*DATOS!$D$9+'COST PER TASK'!J14*'COST PER TASK'!AE14*DATOS!$D$10+'COST PER TASK'!K14*'COST PER TASK'!AE14*DATOS!$D$11+'COST PER TASK'!L14*'COST PER TASK'!AE14*DATOS!$D$12+'COST PER TASK'!M14*'COST PER TASK'!AE14*DATOS!$D$13+'COST PER TASK'!N14*'COST PER TASK'!AE14*DATOS!$D$14+'COST PER TASK'!O14*'COST PER TASK'!AE14*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI14" s="3">
+      <c r="AI14" s="4">
         <f>'COST PER TASK'!P14*'COST PER TASK'!AE14*DATOS!$D$16+'COST PER TASK'!Q14*'COST PER TASK'!AE14*DATOS!$D$17+'COST PER TASK'!R14*'COST PER TASK'!AE14*DATOS!$D$18+'COST PER TASK'!S14*'COST PER TASK'!AE14*DATOS!$D$19+'COST PER TASK'!T14*'COST PER TASK'!AE14*DATOS!$D$20+'COST PER TASK'!U14*'COST PER TASK'!AE14*DATOS!$D$21+'COST PER TASK'!V14*'COST PER TASK'!AE14*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ14" s="4">
+        <f>'COST PER TASK'!W14*'COST PER TASK'!AE14*DATOS!$B$23+'COST PER TASK'!X14*'COST PER TASK'!AE14*DATOS!$B$24+'COST PER TASK'!Y14*'COST PER TASK'!AE14*DATOS!$B$25+'COST PER TASK'!Z14*'COST PER TASK'!AE14*DATOS!$B$26+'COST PER TASK'!AA14*'COST PER TASK'!AE14*DATOS!$B$27+'COST PER TASK'!AB14*'COST PER TASK'!AE14*DATOS!$B$28+'COST PER TASK'!AC14*'COST PER TASK'!AE14*DATOS!$B$29</f>
+        <v>120</v>
+      </c>
       <c r="AK14" s="8">
         <f t="shared" si="1"/>
-        <v>492</v>
+        <v>612</v>
       </c>
       <c r="AL14" s="8">
         <f t="shared" si="2"/>
-        <v>164</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.2">
@@ -2240,21 +2289,25 @@
         <f>AF15*C15*DATOS!$B$3+'COST PER TASK'!AF15*'COST PER TASK'!D15*DATOS!$B$4+'COST PER TASK'!AF15*'COST PER TASK'!E15*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH15" s="3">
+      <c r="AH15" s="4">
         <f>F15*AE15*DATOS!$D$6+'COST PER TASK'!G15*'COST PER TASK'!AE15*DATOS!$D$7+'COST PER TASK'!H15*'COST PER TASK'!AE15*DATOS!$D$8+'COST PER TASK'!I15*'COST PER TASK'!AE15*DATOS!$D$9+'COST PER TASK'!J15*'COST PER TASK'!AE15*DATOS!$D$10+'COST PER TASK'!K15*'COST PER TASK'!AE15*DATOS!$D$11+'COST PER TASK'!L15*'COST PER TASK'!AE15*DATOS!$D$12+'COST PER TASK'!M15*'COST PER TASK'!AE15*DATOS!$D$13+'COST PER TASK'!N15*'COST PER TASK'!AE15*DATOS!$D$14+'COST PER TASK'!O15*'COST PER TASK'!AE15*DATOS!$D$15</f>
         <v>3114.3150832937426</v>
       </c>
-      <c r="AI15" s="3">
+      <c r="AI15" s="4">
         <f>'COST PER TASK'!P15*'COST PER TASK'!AE15*DATOS!$D$16+'COST PER TASK'!Q15*'COST PER TASK'!AE15*DATOS!$D$17+'COST PER TASK'!R15*'COST PER TASK'!AE15*DATOS!$D$18+'COST PER TASK'!S15*'COST PER TASK'!AE15*DATOS!$D$19+'COST PER TASK'!T15*'COST PER TASK'!AE15*DATOS!$D$20+'COST PER TASK'!U15*'COST PER TASK'!AE15*DATOS!$D$21+'COST PER TASK'!V15*'COST PER TASK'!AE15*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ15" s="4">
+        <f>'COST PER TASK'!W15*'COST PER TASK'!AE15*DATOS!$B$23+'COST PER TASK'!X15*'COST PER TASK'!AE15*DATOS!$B$24+'COST PER TASK'!Y15*'COST PER TASK'!AE15*DATOS!$B$25+'COST PER TASK'!Z15*'COST PER TASK'!AE15*DATOS!$B$26+'COST PER TASK'!AA15*'COST PER TASK'!AE15*DATOS!$B$27+'COST PER TASK'!AB15*'COST PER TASK'!AE15*DATOS!$B$28+'COST PER TASK'!AC15*'COST PER TASK'!AE15*DATOS!$B$29</f>
+        <v>35200</v>
+      </c>
       <c r="AK15" s="8">
         <f t="shared" si="1"/>
-        <v>147434.31508329374</v>
+        <v>182634.31508329374</v>
       </c>
       <c r="AL15" s="8">
         <f t="shared" si="2"/>
-        <v>167.5389944128338</v>
+        <v>207.5389944128338</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
@@ -2294,21 +2347,25 @@
         <f>AF16*C16*DATOS!$B$3+'COST PER TASK'!AF16*'COST PER TASK'!D16*DATOS!$B$4+'COST PER TASK'!AF16*'COST PER TASK'!E16*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH16" s="3">
+      <c r="AH16" s="4">
         <f>F16*AE16*DATOS!$D$6+'COST PER TASK'!G16*'COST PER TASK'!AE16*DATOS!$D$7+'COST PER TASK'!H16*'COST PER TASK'!AE16*DATOS!$D$8+'COST PER TASK'!I16*'COST PER TASK'!AE16*DATOS!$D$9+'COST PER TASK'!J16*'COST PER TASK'!AE16*DATOS!$D$10+'COST PER TASK'!K16*'COST PER TASK'!AE16*DATOS!$D$11+'COST PER TASK'!L16*'COST PER TASK'!AE16*DATOS!$D$12+'COST PER TASK'!M16*'COST PER TASK'!AE16*DATOS!$D$13+'COST PER TASK'!N16*'COST PER TASK'!AE16*DATOS!$D$14+'COST PER TASK'!O16*'COST PER TASK'!AE16*DATOS!$D$15</f>
         <v>3114.3150832937426</v>
       </c>
-      <c r="AI16" s="3">
+      <c r="AI16" s="4">
         <f>'COST PER TASK'!P16*'COST PER TASK'!AE16*DATOS!$D$16+'COST PER TASK'!Q16*'COST PER TASK'!AE16*DATOS!$D$17+'COST PER TASK'!R16*'COST PER TASK'!AE16*DATOS!$D$18+'COST PER TASK'!S16*'COST PER TASK'!AE16*DATOS!$D$19+'COST PER TASK'!T16*'COST PER TASK'!AE16*DATOS!$D$20+'COST PER TASK'!U16*'COST PER TASK'!AE16*DATOS!$D$21+'COST PER TASK'!V16*'COST PER TASK'!AE16*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ16" s="4">
+        <f>'COST PER TASK'!W16*'COST PER TASK'!AE16*DATOS!$B$23+'COST PER TASK'!X16*'COST PER TASK'!AE16*DATOS!$B$24+'COST PER TASK'!Y16*'COST PER TASK'!AE16*DATOS!$B$25+'COST PER TASK'!Z16*'COST PER TASK'!AE16*DATOS!$B$26+'COST PER TASK'!AA16*'COST PER TASK'!AE16*DATOS!$B$27+'COST PER TASK'!AB16*'COST PER TASK'!AE16*DATOS!$B$28+'COST PER TASK'!AC16*'COST PER TASK'!AE16*DATOS!$B$29</f>
+        <v>35200</v>
+      </c>
       <c r="AK16" s="8">
         <f t="shared" si="1"/>
-        <v>147434.31508329374</v>
+        <v>182634.31508329374</v>
       </c>
       <c r="AL16" s="8">
         <f t="shared" si="2"/>
-        <v>167.5389944128338</v>
+        <v>207.5389944128338</v>
       </c>
     </row>
     <row r="17" spans="2:38" x14ac:dyDescent="0.2">
@@ -2348,21 +2405,25 @@
         <f>AF17*C17*DATOS!$B$3+'COST PER TASK'!AF17*'COST PER TASK'!D17*DATOS!$B$4+'COST PER TASK'!AF17*'COST PER TASK'!E17*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH17" s="3">
+      <c r="AH17" s="4">
         <f>F17*AE17*DATOS!$D$6+'COST PER TASK'!G17*'COST PER TASK'!AE17*DATOS!$D$7+'COST PER TASK'!H17*'COST PER TASK'!AE17*DATOS!$D$8+'COST PER TASK'!I17*'COST PER TASK'!AE17*DATOS!$D$9+'COST PER TASK'!J17*'COST PER TASK'!AE17*DATOS!$D$10+'COST PER TASK'!K17*'COST PER TASK'!AE17*DATOS!$D$11+'COST PER TASK'!L17*'COST PER TASK'!AE17*DATOS!$D$12+'COST PER TASK'!M17*'COST PER TASK'!AE17*DATOS!$D$13+'COST PER TASK'!N17*'COST PER TASK'!AE17*DATOS!$D$14+'COST PER TASK'!O17*'COST PER TASK'!AE17*DATOS!$D$15</f>
         <v>3114.3150832937426</v>
       </c>
-      <c r="AI17" s="3">
+      <c r="AI17" s="4">
         <f>'COST PER TASK'!P17*'COST PER TASK'!AE17*DATOS!$D$16+'COST PER TASK'!Q17*'COST PER TASK'!AE17*DATOS!$D$17+'COST PER TASK'!R17*'COST PER TASK'!AE17*DATOS!$D$18+'COST PER TASK'!S17*'COST PER TASK'!AE17*DATOS!$D$19+'COST PER TASK'!T17*'COST PER TASK'!AE17*DATOS!$D$20+'COST PER TASK'!U17*'COST PER TASK'!AE17*DATOS!$D$21+'COST PER TASK'!V17*'COST PER TASK'!AE17*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ17" s="4">
+        <f>'COST PER TASK'!W17*'COST PER TASK'!AE17*DATOS!$B$23+'COST PER TASK'!X17*'COST PER TASK'!AE17*DATOS!$B$24+'COST PER TASK'!Y17*'COST PER TASK'!AE17*DATOS!$B$25+'COST PER TASK'!Z17*'COST PER TASK'!AE17*DATOS!$B$26+'COST PER TASK'!AA17*'COST PER TASK'!AE17*DATOS!$B$27+'COST PER TASK'!AB17*'COST PER TASK'!AE17*DATOS!$B$28+'COST PER TASK'!AC17*'COST PER TASK'!AE17*DATOS!$B$29</f>
+        <v>35200</v>
+      </c>
       <c r="AK17" s="8">
         <f t="shared" si="1"/>
-        <v>147434.31508329374</v>
+        <v>182634.31508329374</v>
       </c>
       <c r="AL17" s="8">
         <f t="shared" si="2"/>
-        <v>167.5389944128338</v>
+        <v>207.5389944128338</v>
       </c>
     </row>
     <row r="18" spans="2:38" x14ac:dyDescent="0.2">
@@ -2402,21 +2463,25 @@
         <f>AF18*C18*DATOS!$B$3+'COST PER TASK'!AF18*'COST PER TASK'!D18*DATOS!$B$4+'COST PER TASK'!AF18*'COST PER TASK'!E18*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH18" s="3">
+      <c r="AH18" s="4">
         <f>F18*AE18*DATOS!$D$6+'COST PER TASK'!G18*'COST PER TASK'!AE18*DATOS!$D$7+'COST PER TASK'!H18*'COST PER TASK'!AE18*DATOS!$D$8+'COST PER TASK'!I18*'COST PER TASK'!AE18*DATOS!$D$9+'COST PER TASK'!J18*'COST PER TASK'!AE18*DATOS!$D$10+'COST PER TASK'!K18*'COST PER TASK'!AE18*DATOS!$D$11+'COST PER TASK'!L18*'COST PER TASK'!AE18*DATOS!$D$12+'COST PER TASK'!M18*'COST PER TASK'!AE18*DATOS!$D$13+'COST PER TASK'!N18*'COST PER TASK'!AE18*DATOS!$D$14+'COST PER TASK'!O18*'COST PER TASK'!AE18*DATOS!$D$15</f>
         <v>3114.3150832937426</v>
       </c>
-      <c r="AI18" s="3">
+      <c r="AI18" s="4">
         <f>'COST PER TASK'!P18*'COST PER TASK'!AE18*DATOS!$D$16+'COST PER TASK'!Q18*'COST PER TASK'!AE18*DATOS!$D$17+'COST PER TASK'!R18*'COST PER TASK'!AE18*DATOS!$D$18+'COST PER TASK'!S18*'COST PER TASK'!AE18*DATOS!$D$19+'COST PER TASK'!T18*'COST PER TASK'!AE18*DATOS!$D$20+'COST PER TASK'!U18*'COST PER TASK'!AE18*DATOS!$D$21+'COST PER TASK'!V18*'COST PER TASK'!AE18*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ18" s="4">
+        <f>'COST PER TASK'!W18*'COST PER TASK'!AE18*DATOS!$B$23+'COST PER TASK'!X18*'COST PER TASK'!AE18*DATOS!$B$24+'COST PER TASK'!Y18*'COST PER TASK'!AE18*DATOS!$B$25+'COST PER TASK'!Z18*'COST PER TASK'!AE18*DATOS!$B$26+'COST PER TASK'!AA18*'COST PER TASK'!AE18*DATOS!$B$27+'COST PER TASK'!AB18*'COST PER TASK'!AE18*DATOS!$B$28+'COST PER TASK'!AC18*'COST PER TASK'!AE18*DATOS!$B$29</f>
+        <v>7040</v>
+      </c>
       <c r="AK18" s="8">
         <f t="shared" si="1"/>
-        <v>147434.31508329374</v>
+        <v>154474.31508329374</v>
       </c>
       <c r="AL18" s="8">
         <f t="shared" si="2"/>
-        <v>167.5389944128338</v>
+        <v>175.5389944128338</v>
       </c>
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.2">
@@ -2450,21 +2515,25 @@
         <f>AF19*C19*DATOS!$B$3+'COST PER TASK'!AF19*'COST PER TASK'!D19*DATOS!$B$4+'COST PER TASK'!AF19*'COST PER TASK'!E19*DATOS!$B$5</f>
         <v>144320</v>
       </c>
-      <c r="AH19" s="3">
+      <c r="AH19" s="4">
         <f>F19*AE19*DATOS!$D$6+'COST PER TASK'!G19*'COST PER TASK'!AE19*DATOS!$D$7+'COST PER TASK'!H19*'COST PER TASK'!AE19*DATOS!$D$8+'COST PER TASK'!I19*'COST PER TASK'!AE19*DATOS!$D$9+'COST PER TASK'!J19*'COST PER TASK'!AE19*DATOS!$D$10+'COST PER TASK'!K19*'COST PER TASK'!AE19*DATOS!$D$11+'COST PER TASK'!L19*'COST PER TASK'!AE19*DATOS!$D$12+'COST PER TASK'!M19*'COST PER TASK'!AE19*DATOS!$D$13+'COST PER TASK'!N19*'COST PER TASK'!AE19*DATOS!$D$14+'COST PER TASK'!O19*'COST PER TASK'!AE19*DATOS!$D$15</f>
         <v>4264</v>
       </c>
-      <c r="AI19" s="3">
+      <c r="AI19" s="4">
         <f>'COST PER TASK'!P19*'COST PER TASK'!AE19*DATOS!$D$16+'COST PER TASK'!Q19*'COST PER TASK'!AE19*DATOS!$D$17+'COST PER TASK'!R19*'COST PER TASK'!AE19*DATOS!$D$18+'COST PER TASK'!S19*'COST PER TASK'!AE19*DATOS!$D$19+'COST PER TASK'!T19*'COST PER TASK'!AE19*DATOS!$D$20+'COST PER TASK'!U19*'COST PER TASK'!AE19*DATOS!$D$21+'COST PER TASK'!V19*'COST PER TASK'!AE19*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ19" s="4">
+        <f>'COST PER TASK'!W19*'COST PER TASK'!AE19*DATOS!$B$23+'COST PER TASK'!X19*'COST PER TASK'!AE19*DATOS!$B$24+'COST PER TASK'!Y19*'COST PER TASK'!AE19*DATOS!$B$25+'COST PER TASK'!Z19*'COST PER TASK'!AE19*DATOS!$B$26+'COST PER TASK'!AA19*'COST PER TASK'!AE19*DATOS!$B$27+'COST PER TASK'!AB19*'COST PER TASK'!AE19*DATOS!$B$28+'COST PER TASK'!AC19*'COST PER TASK'!AE19*DATOS!$B$29</f>
+        <v>7040</v>
+      </c>
       <c r="AK19" s="8">
         <f t="shared" si="1"/>
-        <v>148584</v>
+        <v>155624</v>
       </c>
       <c r="AL19" s="8">
         <f t="shared" si="2"/>
-        <v>168.84545454545454</v>
+        <v>176.84545454545454</v>
       </c>
     </row>
     <row r="20" spans="2:38" x14ac:dyDescent="0.2">
@@ -2507,21 +2576,25 @@
         <f>AF20*C20*DATOS!$B$3+'COST PER TASK'!AF20*'COST PER TASK'!D20*DATOS!$B$4+'COST PER TASK'!AF20*'COST PER TASK'!E20*DATOS!$B$5</f>
         <v>3984</v>
       </c>
-      <c r="AH20" s="3">
+      <c r="AH20" s="4">
         <f>F20*AE20*DATOS!$D$6+'COST PER TASK'!G20*'COST PER TASK'!AE20*DATOS!$D$7+'COST PER TASK'!H20*'COST PER TASK'!AE20*DATOS!$D$8+'COST PER TASK'!I20*'COST PER TASK'!AE20*DATOS!$D$9+'COST PER TASK'!J20*'COST PER TASK'!AE20*DATOS!$D$10+'COST PER TASK'!K20*'COST PER TASK'!AE20*DATOS!$D$11+'COST PER TASK'!L20*'COST PER TASK'!AE20*DATOS!$D$12+'COST PER TASK'!M20*'COST PER TASK'!AE20*DATOS!$D$13+'COST PER TASK'!N20*'COST PER TASK'!AE20*DATOS!$D$14+'COST PER TASK'!O20*'COST PER TASK'!AE20*DATOS!$D$15</f>
         <v>106.16983238501395</v>
       </c>
-      <c r="AI20" s="3">
+      <c r="AI20" s="4">
         <f>'COST PER TASK'!P20*'COST PER TASK'!AE20*DATOS!$D$16+'COST PER TASK'!Q20*'COST PER TASK'!AE20*DATOS!$D$17+'COST PER TASK'!R20*'COST PER TASK'!AE20*DATOS!$D$18+'COST PER TASK'!S20*'COST PER TASK'!AE20*DATOS!$D$19+'COST PER TASK'!T20*'COST PER TASK'!AE20*DATOS!$D$20+'COST PER TASK'!U20*'COST PER TASK'!AE20*DATOS!$D$21+'COST PER TASK'!V20*'COST PER TASK'!AE20*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ20" s="4">
+        <f>'COST PER TASK'!W20*'COST PER TASK'!AE20*DATOS!$B$23+'COST PER TASK'!X20*'COST PER TASK'!AE20*DATOS!$B$24+'COST PER TASK'!Y20*'COST PER TASK'!AE20*DATOS!$B$25+'COST PER TASK'!Z20*'COST PER TASK'!AE20*DATOS!$B$26+'COST PER TASK'!AA20*'COST PER TASK'!AE20*DATOS!$B$27+'COST PER TASK'!AB20*'COST PER TASK'!AE20*DATOS!$B$28+'COST PER TASK'!AC20*'COST PER TASK'!AE20*DATOS!$B$29</f>
+        <v>1200</v>
+      </c>
       <c r="AK20" s="8">
         <f t="shared" si="1"/>
-        <v>4090.1698323850142</v>
+        <v>5290.1698323850142</v>
       </c>
       <c r="AL20" s="8">
         <f t="shared" si="2"/>
-        <v>136.33899441283381</v>
+        <v>176.33899441283381</v>
       </c>
     </row>
     <row r="21" spans="2:38" x14ac:dyDescent="0.2">
@@ -2561,21 +2634,25 @@
         <f>AF21*C21*DATOS!$B$3+'COST PER TASK'!AF21*'COST PER TASK'!D21*DATOS!$B$4+'COST PER TASK'!AF21*'COST PER TASK'!E21*DATOS!$B$5</f>
         <v>3800</v>
       </c>
-      <c r="AH21" s="3">
+      <c r="AH21" s="4">
         <f>F21*AE21*DATOS!$D$6+'COST PER TASK'!G21*'COST PER TASK'!AE21*DATOS!$D$7+'COST PER TASK'!H21*'COST PER TASK'!AE21*DATOS!$D$8+'COST PER TASK'!I21*'COST PER TASK'!AE21*DATOS!$D$9+'COST PER TASK'!J21*'COST PER TASK'!AE21*DATOS!$D$10+'COST PER TASK'!K21*'COST PER TASK'!AE21*DATOS!$D$11+'COST PER TASK'!L21*'COST PER TASK'!AE21*DATOS!$D$12+'COST PER TASK'!M21*'COST PER TASK'!AE21*DATOS!$D$13+'COST PER TASK'!N21*'COST PER TASK'!AE21*DATOS!$D$14+'COST PER TASK'!O21*'COST PER TASK'!AE21*DATOS!$D$15</f>
         <v>88.474860320844954</v>
       </c>
-      <c r="AI21" s="3">
+      <c r="AI21" s="4">
         <f>'COST PER TASK'!P21*'COST PER TASK'!AE21*DATOS!$D$16+'COST PER TASK'!Q21*'COST PER TASK'!AE21*DATOS!$D$17+'COST PER TASK'!R21*'COST PER TASK'!AE21*DATOS!$D$18+'COST PER TASK'!S21*'COST PER TASK'!AE21*DATOS!$D$19+'COST PER TASK'!T21*'COST PER TASK'!AE21*DATOS!$D$20+'COST PER TASK'!U21*'COST PER TASK'!AE21*DATOS!$D$21+'COST PER TASK'!V21*'COST PER TASK'!AE21*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ21" s="4">
+        <f>'COST PER TASK'!W21*'COST PER TASK'!AE21*DATOS!$B$23+'COST PER TASK'!X21*'COST PER TASK'!AE21*DATOS!$B$24+'COST PER TASK'!Y21*'COST PER TASK'!AE21*DATOS!$B$25+'COST PER TASK'!Z21*'COST PER TASK'!AE21*DATOS!$B$26+'COST PER TASK'!AA21*'COST PER TASK'!AE21*DATOS!$B$27+'COST PER TASK'!AB21*'COST PER TASK'!AE21*DATOS!$B$28+'COST PER TASK'!AC21*'COST PER TASK'!AE21*DATOS!$B$29</f>
+        <v>1000</v>
+      </c>
       <c r="AK21" s="8">
         <f t="shared" si="1"/>
-        <v>3888.474860320845</v>
+        <v>4888.4748603208445</v>
       </c>
       <c r="AL21" s="8">
         <f t="shared" si="2"/>
-        <v>155.5389944128338</v>
+        <v>195.53899441283377</v>
       </c>
     </row>
     <row r="22" spans="2:38" x14ac:dyDescent="0.2">
@@ -2618,21 +2695,25 @@
         <f>AF22*C22*DATOS!$B$3+'COST PER TASK'!AF22*'COST PER TASK'!D22*DATOS!$B$4+'COST PER TASK'!AF22*'COST PER TASK'!E22*DATOS!$B$5</f>
         <v>3320</v>
       </c>
-      <c r="AH22" s="3">
+      <c r="AH22" s="4">
         <f>F22*AE22*DATOS!$D$6+'COST PER TASK'!G22*'COST PER TASK'!AE22*DATOS!$D$7+'COST PER TASK'!H22*'COST PER TASK'!AE22*DATOS!$D$8+'COST PER TASK'!I22*'COST PER TASK'!AE22*DATOS!$D$9+'COST PER TASK'!J22*'COST PER TASK'!AE22*DATOS!$D$10+'COST PER TASK'!K22*'COST PER TASK'!AE22*DATOS!$D$11+'COST PER TASK'!L22*'COST PER TASK'!AE22*DATOS!$D$12+'COST PER TASK'!M22*'COST PER TASK'!AE22*DATOS!$D$13+'COST PER TASK'!N22*'COST PER TASK'!AE22*DATOS!$D$14+'COST PER TASK'!O22*'COST PER TASK'!AE22*DATOS!$D$15</f>
         <v>88.474860320844954</v>
       </c>
-      <c r="AI22" s="3">
+      <c r="AI22" s="4">
         <f>'COST PER TASK'!P22*'COST PER TASK'!AE22*DATOS!$D$16+'COST PER TASK'!Q22*'COST PER TASK'!AE22*DATOS!$D$17+'COST PER TASK'!R22*'COST PER TASK'!AE22*DATOS!$D$18+'COST PER TASK'!S22*'COST PER TASK'!AE22*DATOS!$D$19+'COST PER TASK'!T22*'COST PER TASK'!AE22*DATOS!$D$20+'COST PER TASK'!U22*'COST PER TASK'!AE22*DATOS!$D$21+'COST PER TASK'!V22*'COST PER TASK'!AE22*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ22" s="4">
+        <f>'COST PER TASK'!W22*'COST PER TASK'!AE22*DATOS!$B$23+'COST PER TASK'!X22*'COST PER TASK'!AE22*DATOS!$B$24+'COST PER TASK'!Y22*'COST PER TASK'!AE22*DATOS!$B$25+'COST PER TASK'!Z22*'COST PER TASK'!AE22*DATOS!$B$26+'COST PER TASK'!AA22*'COST PER TASK'!AE22*DATOS!$B$27+'COST PER TASK'!AB22*'COST PER TASK'!AE22*DATOS!$B$28+'COST PER TASK'!AC22*'COST PER TASK'!AE22*DATOS!$B$29</f>
+        <v>1000</v>
+      </c>
       <c r="AK22" s="8">
         <f t="shared" si="1"/>
-        <v>3408.474860320845</v>
+        <v>4408.4748603208445</v>
       </c>
       <c r="AL22" s="8">
         <f t="shared" si="2"/>
-        <v>136.33899441283381</v>
+        <v>176.33899441283378</v>
       </c>
     </row>
     <row r="23" spans="2:38" x14ac:dyDescent="0.2">
@@ -2672,21 +2753,25 @@
         <f>AF23*C23*DATOS!$B$3+'COST PER TASK'!AF23*'COST PER TASK'!D23*DATOS!$B$4+'COST PER TASK'!AF23*'COST PER TASK'!E23*DATOS!$B$5</f>
         <v>4560</v>
       </c>
-      <c r="AH23" s="3">
+      <c r="AH23" s="4">
         <f>F23*AE23*DATOS!$D$6+'COST PER TASK'!G23*'COST PER TASK'!AE23*DATOS!$D$7+'COST PER TASK'!H23*'COST PER TASK'!AE23*DATOS!$D$8+'COST PER TASK'!I23*'COST PER TASK'!AE23*DATOS!$D$9+'COST PER TASK'!J23*'COST PER TASK'!AE23*DATOS!$D$10+'COST PER TASK'!K23*'COST PER TASK'!AE23*DATOS!$D$11+'COST PER TASK'!L23*'COST PER TASK'!AE23*DATOS!$D$12+'COST PER TASK'!M23*'COST PER TASK'!AE23*DATOS!$D$13+'COST PER TASK'!N23*'COST PER TASK'!AE23*DATOS!$D$14+'COST PER TASK'!O23*'COST PER TASK'!AE23*DATOS!$D$15</f>
         <v>106.16983238501395</v>
       </c>
-      <c r="AI23" s="3">
+      <c r="AI23" s="4">
         <f>'COST PER TASK'!P23*'COST PER TASK'!AE23*DATOS!$D$16+'COST PER TASK'!Q23*'COST PER TASK'!AE23*DATOS!$D$17+'COST PER TASK'!R23*'COST PER TASK'!AE23*DATOS!$D$18+'COST PER TASK'!S23*'COST PER TASK'!AE23*DATOS!$D$19+'COST PER TASK'!T23*'COST PER TASK'!AE23*DATOS!$D$20+'COST PER TASK'!U23*'COST PER TASK'!AE23*DATOS!$D$21+'COST PER TASK'!V23*'COST PER TASK'!AE23*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ23" s="4">
+        <f>'COST PER TASK'!W23*'COST PER TASK'!AE23*DATOS!$B$23+'COST PER TASK'!X23*'COST PER TASK'!AE23*DATOS!$B$24+'COST PER TASK'!Y23*'COST PER TASK'!AE23*DATOS!$B$25+'COST PER TASK'!Z23*'COST PER TASK'!AE23*DATOS!$B$26+'COST PER TASK'!AA23*'COST PER TASK'!AE23*DATOS!$B$27+'COST PER TASK'!AB23*'COST PER TASK'!AE23*DATOS!$B$28+'COST PER TASK'!AC23*'COST PER TASK'!AE23*DATOS!$B$29</f>
+        <v>1200</v>
+      </c>
       <c r="AK23" s="8">
         <f t="shared" si="1"/>
-        <v>4666.1698323850142</v>
+        <v>5866.1698323850142</v>
       </c>
       <c r="AL23" s="8">
         <f t="shared" si="2"/>
-        <v>155.5389944128338</v>
+        <v>195.5389944128338</v>
       </c>
     </row>
     <row r="24" spans="2:38" x14ac:dyDescent="0.2">
@@ -2729,21 +2814,25 @@
         <f>AF24*C24*DATOS!$B$3+'COST PER TASK'!AF24*'COST PER TASK'!D24*DATOS!$B$4+'COST PER TASK'!AF24*'COST PER TASK'!E24*DATOS!$B$5</f>
         <v>2656</v>
       </c>
-      <c r="AH24" s="3">
+      <c r="AH24" s="4">
         <f>F24*AE24*DATOS!$D$6+'COST PER TASK'!G24*'COST PER TASK'!AE24*DATOS!$D$7+'COST PER TASK'!H24*'COST PER TASK'!AE24*DATOS!$D$8+'COST PER TASK'!I24*'COST PER TASK'!AE24*DATOS!$D$9+'COST PER TASK'!J24*'COST PER TASK'!AE24*DATOS!$D$10+'COST PER TASK'!K24*'COST PER TASK'!AE24*DATOS!$D$11+'COST PER TASK'!L24*'COST PER TASK'!AE24*DATOS!$D$12+'COST PER TASK'!M24*'COST PER TASK'!AE24*DATOS!$D$13+'COST PER TASK'!N24*'COST PER TASK'!AE24*DATOS!$D$14+'COST PER TASK'!O24*'COST PER TASK'!AE24*DATOS!$D$15</f>
         <v>70.77988825667596</v>
       </c>
-      <c r="AI24" s="3">
+      <c r="AI24" s="4">
         <f>'COST PER TASK'!P24*'COST PER TASK'!AE24*DATOS!$D$16+'COST PER TASK'!Q24*'COST PER TASK'!AE24*DATOS!$D$17+'COST PER TASK'!R24*'COST PER TASK'!AE24*DATOS!$D$18+'COST PER TASK'!S24*'COST PER TASK'!AE24*DATOS!$D$19+'COST PER TASK'!T24*'COST PER TASK'!AE24*DATOS!$D$20+'COST PER TASK'!U24*'COST PER TASK'!AE24*DATOS!$D$21+'COST PER TASK'!V24*'COST PER TASK'!AE24*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ24" s="4">
+        <f>'COST PER TASK'!W24*'COST PER TASK'!AE24*DATOS!$B$23+'COST PER TASK'!X24*'COST PER TASK'!AE24*DATOS!$B$24+'COST PER TASK'!Y24*'COST PER TASK'!AE24*DATOS!$B$25+'COST PER TASK'!Z24*'COST PER TASK'!AE24*DATOS!$B$26+'COST PER TASK'!AA24*'COST PER TASK'!AE24*DATOS!$B$27+'COST PER TASK'!AB24*'COST PER TASK'!AE24*DATOS!$B$28+'COST PER TASK'!AC24*'COST PER TASK'!AE24*DATOS!$B$29</f>
+        <v>800</v>
+      </c>
       <c r="AK24" s="8">
         <f t="shared" si="1"/>
-        <v>2726.7798882566758</v>
+        <v>3526.7798882566758</v>
       </c>
       <c r="AL24" s="8">
         <f t="shared" si="2"/>
-        <v>136.33899441283378</v>
+        <v>176.33899441283378</v>
       </c>
     </row>
     <row r="25" spans="2:38" x14ac:dyDescent="0.2">
@@ -2786,21 +2875,25 @@
         <f>AF25*C25*DATOS!$B$3+'COST PER TASK'!AF25*'COST PER TASK'!D25*DATOS!$B$4+'COST PER TASK'!AF25*'COST PER TASK'!E25*DATOS!$B$5</f>
         <v>2656</v>
       </c>
-      <c r="AH25" s="3">
+      <c r="AH25" s="4">
         <f>F25*AE25*DATOS!$D$6+'COST PER TASK'!G25*'COST PER TASK'!AE25*DATOS!$D$7+'COST PER TASK'!H25*'COST PER TASK'!AE25*DATOS!$D$8+'COST PER TASK'!I25*'COST PER TASK'!AE25*DATOS!$D$9+'COST PER TASK'!J25*'COST PER TASK'!AE25*DATOS!$D$10+'COST PER TASK'!K25*'COST PER TASK'!AE25*DATOS!$D$11+'COST PER TASK'!L25*'COST PER TASK'!AE25*DATOS!$D$12+'COST PER TASK'!M25*'COST PER TASK'!AE25*DATOS!$D$13+'COST PER TASK'!N25*'COST PER TASK'!AE25*DATOS!$D$14+'COST PER TASK'!O25*'COST PER TASK'!AE25*DATOS!$D$15</f>
         <v>70.77988825667596</v>
       </c>
-      <c r="AI25" s="3">
+      <c r="AI25" s="4">
         <f>'COST PER TASK'!P25*'COST PER TASK'!AE25*DATOS!$D$16+'COST PER TASK'!Q25*'COST PER TASK'!AE25*DATOS!$D$17+'COST PER TASK'!R25*'COST PER TASK'!AE25*DATOS!$D$18+'COST PER TASK'!S25*'COST PER TASK'!AE25*DATOS!$D$19+'COST PER TASK'!T25*'COST PER TASK'!AE25*DATOS!$D$20+'COST PER TASK'!U25*'COST PER TASK'!AE25*DATOS!$D$21+'COST PER TASK'!V25*'COST PER TASK'!AE25*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ25" s="4">
+        <f>'COST PER TASK'!W25*'COST PER TASK'!AE25*DATOS!$B$23+'COST PER TASK'!X25*'COST PER TASK'!AE25*DATOS!$B$24+'COST PER TASK'!Y25*'COST PER TASK'!AE25*DATOS!$B$25+'COST PER TASK'!Z25*'COST PER TASK'!AE25*DATOS!$B$26+'COST PER TASK'!AA25*'COST PER TASK'!AE25*DATOS!$B$27+'COST PER TASK'!AB25*'COST PER TASK'!AE25*DATOS!$B$28+'COST PER TASK'!AC25*'COST PER TASK'!AE25*DATOS!$B$29</f>
+        <v>800</v>
+      </c>
       <c r="AK25" s="8">
         <f t="shared" si="1"/>
-        <v>2726.7798882566758</v>
+        <v>3526.7798882566758</v>
       </c>
       <c r="AL25" s="8">
         <f t="shared" si="2"/>
-        <v>136.33899441283378</v>
+        <v>176.33899441283378</v>
       </c>
     </row>
     <row r="26" spans="2:38" x14ac:dyDescent="0.2">
@@ -2843,21 +2936,25 @@
         <f>AF26*C26*DATOS!$B$3+'COST PER TASK'!AF26*'COST PER TASK'!D26*DATOS!$B$4+'COST PER TASK'!AF26*'COST PER TASK'!E26*DATOS!$B$5</f>
         <v>2656</v>
       </c>
-      <c r="AH26" s="3">
+      <c r="AH26" s="4">
         <f>F26*AE26*DATOS!$D$6+'COST PER TASK'!G26*'COST PER TASK'!AE26*DATOS!$D$7+'COST PER TASK'!H26*'COST PER TASK'!AE26*DATOS!$D$8+'COST PER TASK'!I26*'COST PER TASK'!AE26*DATOS!$D$9+'COST PER TASK'!J26*'COST PER TASK'!AE26*DATOS!$D$10+'COST PER TASK'!K26*'COST PER TASK'!AE26*DATOS!$D$11+'COST PER TASK'!L26*'COST PER TASK'!AE26*DATOS!$D$12+'COST PER TASK'!M26*'COST PER TASK'!AE26*DATOS!$D$13+'COST PER TASK'!N26*'COST PER TASK'!AE26*DATOS!$D$14+'COST PER TASK'!O26*'COST PER TASK'!AE26*DATOS!$D$15</f>
         <v>70.77988825667596</v>
       </c>
-      <c r="AI26" s="3">
+      <c r="AI26" s="4">
         <f>'COST PER TASK'!P26*'COST PER TASK'!AE26*DATOS!$D$16+'COST PER TASK'!Q26*'COST PER TASK'!AE26*DATOS!$D$17+'COST PER TASK'!R26*'COST PER TASK'!AE26*DATOS!$D$18+'COST PER TASK'!S26*'COST PER TASK'!AE26*DATOS!$D$19+'COST PER TASK'!T26*'COST PER TASK'!AE26*DATOS!$D$20+'COST PER TASK'!U26*'COST PER TASK'!AE26*DATOS!$D$21+'COST PER TASK'!V26*'COST PER TASK'!AE26*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ26" s="4">
+        <f>'COST PER TASK'!W26*'COST PER TASK'!AE26*DATOS!$B$23+'COST PER TASK'!X26*'COST PER TASK'!AE26*DATOS!$B$24+'COST PER TASK'!Y26*'COST PER TASK'!AE26*DATOS!$B$25+'COST PER TASK'!Z26*'COST PER TASK'!AE26*DATOS!$B$26+'COST PER TASK'!AA26*'COST PER TASK'!AE26*DATOS!$B$27+'COST PER TASK'!AB26*'COST PER TASK'!AE26*DATOS!$B$28+'COST PER TASK'!AC26*'COST PER TASK'!AE26*DATOS!$B$29</f>
+        <v>800</v>
+      </c>
       <c r="AK26" s="8">
         <f t="shared" si="1"/>
-        <v>2726.7798882566758</v>
+        <v>3526.7798882566758</v>
       </c>
       <c r="AL26" s="8">
         <f t="shared" si="2"/>
-        <v>136.33899441283378</v>
+        <v>176.33899441283378</v>
       </c>
     </row>
     <row r="27" spans="2:38" x14ac:dyDescent="0.2">
@@ -2897,21 +2994,25 @@
         <f>AF27*C27*DATOS!$B$3+'COST PER TASK'!AF27*'COST PER TASK'!D27*DATOS!$B$4+'COST PER TASK'!AF27*'COST PER TASK'!E27*DATOS!$B$5</f>
         <v>6080</v>
       </c>
-      <c r="AH27" s="3">
+      <c r="AH27" s="4">
         <f>F27*AE27*DATOS!$D$6+'COST PER TASK'!G27*'COST PER TASK'!AE27*DATOS!$D$7+'COST PER TASK'!H27*'COST PER TASK'!AE27*DATOS!$D$8+'COST PER TASK'!I27*'COST PER TASK'!AE27*DATOS!$D$9+'COST PER TASK'!J27*'COST PER TASK'!AE27*DATOS!$D$10+'COST PER TASK'!K27*'COST PER TASK'!AE27*DATOS!$D$11+'COST PER TASK'!L27*'COST PER TASK'!AE27*DATOS!$D$12+'COST PER TASK'!M27*'COST PER TASK'!AE27*DATOS!$D$13+'COST PER TASK'!N27*'COST PER TASK'!AE27*DATOS!$D$14+'COST PER TASK'!O27*'COST PER TASK'!AE27*DATOS!$D$15</f>
         <v>141.55977651335192</v>
       </c>
-      <c r="AI27" s="3">
+      <c r="AI27" s="4">
         <f>'COST PER TASK'!P27*'COST PER TASK'!AE27*DATOS!$D$16+'COST PER TASK'!Q27*'COST PER TASK'!AE27*DATOS!$D$17+'COST PER TASK'!R27*'COST PER TASK'!AE27*DATOS!$D$18+'COST PER TASK'!S27*'COST PER TASK'!AE27*DATOS!$D$19+'COST PER TASK'!T27*'COST PER TASK'!AE27*DATOS!$D$20+'COST PER TASK'!U27*'COST PER TASK'!AE27*DATOS!$D$21+'COST PER TASK'!V27*'COST PER TASK'!AE27*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ27" s="4">
+        <f>'COST PER TASK'!W27*'COST PER TASK'!AE27*DATOS!$B$23+'COST PER TASK'!X27*'COST PER TASK'!AE27*DATOS!$B$24+'COST PER TASK'!Y27*'COST PER TASK'!AE27*DATOS!$B$25+'COST PER TASK'!Z27*'COST PER TASK'!AE27*DATOS!$B$26+'COST PER TASK'!AA27*'COST PER TASK'!AE27*DATOS!$B$27+'COST PER TASK'!AB27*'COST PER TASK'!AE27*DATOS!$B$28+'COST PER TASK'!AC27*'COST PER TASK'!AE27*DATOS!$B$29</f>
+        <v>1600</v>
+      </c>
       <c r="AK27" s="8">
         <f t="shared" si="1"/>
-        <v>6221.5597765133516</v>
+        <v>7821.5597765133516</v>
       </c>
       <c r="AL27" s="8">
         <f t="shared" si="2"/>
-        <v>155.5389944128338</v>
+        <v>195.5389944128338</v>
       </c>
     </row>
     <row r="28" spans="2:38" x14ac:dyDescent="0.2">
@@ -2954,21 +3055,25 @@
         <f>AF28*C28*DATOS!$B$3+'COST PER TASK'!AF28*'COST PER TASK'!D28*DATOS!$B$4+'COST PER TASK'!AF28*'COST PER TASK'!E28*DATOS!$B$5</f>
         <v>4380</v>
       </c>
-      <c r="AH28" s="3">
+      <c r="AH28" s="4">
         <f>F28*AE28*DATOS!$D$6+'COST PER TASK'!G28*'COST PER TASK'!AE28*DATOS!$D$7+'COST PER TASK'!H28*'COST PER TASK'!AE28*DATOS!$D$8+'COST PER TASK'!I28*'COST PER TASK'!AE28*DATOS!$D$9+'COST PER TASK'!J28*'COST PER TASK'!AE28*DATOS!$D$10+'COST PER TASK'!K28*'COST PER TASK'!AE28*DATOS!$D$11+'COST PER TASK'!L28*'COST PER TASK'!AE28*DATOS!$D$12+'COST PER TASK'!M28*'COST PER TASK'!AE28*DATOS!$D$13+'COST PER TASK'!N28*'COST PER TASK'!AE28*DATOS!$D$14+'COST PER TASK'!O28*'COST PER TASK'!AE28*DATOS!$D$15</f>
         <v>421.00129305917125</v>
       </c>
-      <c r="AI28" s="3">
+      <c r="AI28" s="4">
         <f>'COST PER TASK'!P28*'COST PER TASK'!AE28*DATOS!$D$16+'COST PER TASK'!Q28*'COST PER TASK'!AE28*DATOS!$D$17+'COST PER TASK'!R28*'COST PER TASK'!AE28*DATOS!$D$18+'COST PER TASK'!S28*'COST PER TASK'!AE28*DATOS!$D$19+'COST PER TASK'!T28*'COST PER TASK'!AE28*DATOS!$D$20+'COST PER TASK'!U28*'COST PER TASK'!AE28*DATOS!$D$21+'COST PER TASK'!V28*'COST PER TASK'!AE28*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ28" s="4">
+        <f>'COST PER TASK'!W28*'COST PER TASK'!AE28*DATOS!$B$23+'COST PER TASK'!X28*'COST PER TASK'!AE28*DATOS!$B$24+'COST PER TASK'!Y28*'COST PER TASK'!AE28*DATOS!$B$25+'COST PER TASK'!Z28*'COST PER TASK'!AE28*DATOS!$B$26+'COST PER TASK'!AA28*'COST PER TASK'!AE28*DATOS!$B$27+'COST PER TASK'!AB28*'COST PER TASK'!AE28*DATOS!$B$28+'COST PER TASK'!AC28*'COST PER TASK'!AE28*DATOS!$B$29</f>
+        <v>16800</v>
+      </c>
       <c r="AK28" s="8">
         <f t="shared" si="1"/>
-        <v>4801.0012930591711</v>
+        <v>21601.001293059169</v>
       </c>
       <c r="AL28" s="8">
         <f t="shared" si="2"/>
-        <v>160.03337643530571</v>
+        <v>720.03337643530563</v>
       </c>
     </row>
     <row r="29" spans="2:38" x14ac:dyDescent="0.2">
@@ -3014,21 +3119,25 @@
         <f>AF29*C29*DATOS!$B$3+'COST PER TASK'!AF29*'COST PER TASK'!D29*DATOS!$B$4+'COST PER TASK'!AF29*'COST PER TASK'!E29*DATOS!$B$5</f>
         <v>6571.4285714285725</v>
       </c>
-      <c r="AH29" s="3">
+      <c r="AH29" s="4">
         <f>F29*AE29*DATOS!$D$6+'COST PER TASK'!G29*'COST PER TASK'!AE29*DATOS!$D$7+'COST PER TASK'!H29*'COST PER TASK'!AE29*DATOS!$D$8+'COST PER TASK'!I29*'COST PER TASK'!AE29*DATOS!$D$9+'COST PER TASK'!J29*'COST PER TASK'!AE29*DATOS!$D$10+'COST PER TASK'!K29*'COST PER TASK'!AE29*DATOS!$D$11+'COST PER TASK'!L29*'COST PER TASK'!AE29*DATOS!$D$12+'COST PER TASK'!M29*'COST PER TASK'!AE29*DATOS!$D$13+'COST PER TASK'!N29*'COST PER TASK'!AE29*DATOS!$D$14+'COST PER TASK'!O29*'COST PER TASK'!AE29*DATOS!$D$15</f>
         <v>701.66882176528543</v>
       </c>
-      <c r="AI29" s="3">
+      <c r="AI29" s="4">
         <f>'COST PER TASK'!P29*'COST PER TASK'!AE29*DATOS!$D$16+'COST PER TASK'!Q29*'COST PER TASK'!AE29*DATOS!$D$17+'COST PER TASK'!R29*'COST PER TASK'!AE29*DATOS!$D$18+'COST PER TASK'!S29*'COST PER TASK'!AE29*DATOS!$D$19+'COST PER TASK'!T29*'COST PER TASK'!AE29*DATOS!$D$20+'COST PER TASK'!U29*'COST PER TASK'!AE29*DATOS!$D$21+'COST PER TASK'!V29*'COST PER TASK'!AE29*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ29" s="4">
+        <f>'COST PER TASK'!W29*'COST PER TASK'!AE29*DATOS!$B$23+'COST PER TASK'!X29*'COST PER TASK'!AE29*DATOS!$B$24+'COST PER TASK'!Y29*'COST PER TASK'!AE29*DATOS!$B$25+'COST PER TASK'!Z29*'COST PER TASK'!AE29*DATOS!$B$26+'COST PER TASK'!AA29*'COST PER TASK'!AE29*DATOS!$B$27+'COST PER TASK'!AB29*'COST PER TASK'!AE29*DATOS!$B$28+'COST PER TASK'!AC29*'COST PER TASK'!AE29*DATOS!$B$29</f>
+        <v>20000</v>
+      </c>
       <c r="AK29" s="8">
         <f t="shared" si="1"/>
-        <v>7273.0973931938579</v>
+        <v>27273.097393193857</v>
       </c>
       <c r="AL29" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387716</v>
+        <v>545.46194786387719</v>
       </c>
     </row>
     <row r="30" spans="2:38" x14ac:dyDescent="0.2">
@@ -3074,21 +3183,25 @@
         <f>AF30*C30*DATOS!$B$3+'COST PER TASK'!AF30*'COST PER TASK'!D30*DATOS!$B$4+'COST PER TASK'!AF30*'COST PER TASK'!E30*DATOS!$B$5</f>
         <v>3942.8571428571431</v>
       </c>
-      <c r="AH30" s="3">
+      <c r="AH30" s="4">
         <f>F30*AE30*DATOS!$D$6+'COST PER TASK'!G30*'COST PER TASK'!AE30*DATOS!$D$7+'COST PER TASK'!H30*'COST PER TASK'!AE30*DATOS!$D$8+'COST PER TASK'!I30*'COST PER TASK'!AE30*DATOS!$D$9+'COST PER TASK'!J30*'COST PER TASK'!AE30*DATOS!$D$10+'COST PER TASK'!K30*'COST PER TASK'!AE30*DATOS!$D$11+'COST PER TASK'!L30*'COST PER TASK'!AE30*DATOS!$D$12+'COST PER TASK'!M30*'COST PER TASK'!AE30*DATOS!$D$13+'COST PER TASK'!N30*'COST PER TASK'!AE30*DATOS!$D$14+'COST PER TASK'!O30*'COST PER TASK'!AE30*DATOS!$D$15</f>
         <v>421.00129305917125</v>
       </c>
-      <c r="AI30" s="3">
+      <c r="AI30" s="4">
         <f>'COST PER TASK'!P30*'COST PER TASK'!AE30*DATOS!$D$16+'COST PER TASK'!Q30*'COST PER TASK'!AE30*DATOS!$D$17+'COST PER TASK'!R30*'COST PER TASK'!AE30*DATOS!$D$18+'COST PER TASK'!S30*'COST PER TASK'!AE30*DATOS!$D$19+'COST PER TASK'!T30*'COST PER TASK'!AE30*DATOS!$D$20+'COST PER TASK'!U30*'COST PER TASK'!AE30*DATOS!$D$21+'COST PER TASK'!V30*'COST PER TASK'!AE30*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ30" s="4">
+        <f>'COST PER TASK'!W30*'COST PER TASK'!AE30*DATOS!$B$23+'COST PER TASK'!X30*'COST PER TASK'!AE30*DATOS!$B$24+'COST PER TASK'!Y30*'COST PER TASK'!AE30*DATOS!$B$25+'COST PER TASK'!Z30*'COST PER TASK'!AE30*DATOS!$B$26+'COST PER TASK'!AA30*'COST PER TASK'!AE30*DATOS!$B$27+'COST PER TASK'!AB30*'COST PER TASK'!AE30*DATOS!$B$28+'COST PER TASK'!AC30*'COST PER TASK'!AE30*DATOS!$B$29</f>
+        <v>2400</v>
+      </c>
       <c r="AK30" s="8">
         <f t="shared" si="1"/>
-        <v>4363.8584359163142</v>
+        <v>6763.8584359163142</v>
       </c>
       <c r="AL30" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387713</v>
+        <v>225.46194786387713</v>
       </c>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.2">
@@ -3134,21 +3247,25 @@
         <f>AF31*C31*DATOS!$B$3+'COST PER TASK'!AF31*'COST PER TASK'!D31*DATOS!$B$4+'COST PER TASK'!AF31*'COST PER TASK'!E31*DATOS!$B$5</f>
         <v>3942.8571428571431</v>
       </c>
-      <c r="AH31" s="3">
+      <c r="AH31" s="4">
         <f>F31*AE31*DATOS!$D$6+'COST PER TASK'!G31*'COST PER TASK'!AE31*DATOS!$D$7+'COST PER TASK'!H31*'COST PER TASK'!AE31*DATOS!$D$8+'COST PER TASK'!I31*'COST PER TASK'!AE31*DATOS!$D$9+'COST PER TASK'!J31*'COST PER TASK'!AE31*DATOS!$D$10+'COST PER TASK'!K31*'COST PER TASK'!AE31*DATOS!$D$11+'COST PER TASK'!L31*'COST PER TASK'!AE31*DATOS!$D$12+'COST PER TASK'!M31*'COST PER TASK'!AE31*DATOS!$D$13+'COST PER TASK'!N31*'COST PER TASK'!AE31*DATOS!$D$14+'COST PER TASK'!O31*'COST PER TASK'!AE31*DATOS!$D$15</f>
         <v>421.00129305917125</v>
       </c>
-      <c r="AI31" s="3">
+      <c r="AI31" s="4">
         <f>'COST PER TASK'!P31*'COST PER TASK'!AE31*DATOS!$D$16+'COST PER TASK'!Q31*'COST PER TASK'!AE31*DATOS!$D$17+'COST PER TASK'!R31*'COST PER TASK'!AE31*DATOS!$D$18+'COST PER TASK'!S31*'COST PER TASK'!AE31*DATOS!$D$19+'COST PER TASK'!T31*'COST PER TASK'!AE31*DATOS!$D$20+'COST PER TASK'!U31*'COST PER TASK'!AE31*DATOS!$D$21+'COST PER TASK'!V31*'COST PER TASK'!AE31*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ31" s="4">
+        <f>'COST PER TASK'!W31*'COST PER TASK'!AE31*DATOS!$B$23+'COST PER TASK'!X31*'COST PER TASK'!AE31*DATOS!$B$24+'COST PER TASK'!Y31*'COST PER TASK'!AE31*DATOS!$B$25+'COST PER TASK'!Z31*'COST PER TASK'!AE31*DATOS!$B$26+'COST PER TASK'!AA31*'COST PER TASK'!AE31*DATOS!$B$27+'COST PER TASK'!AB31*'COST PER TASK'!AE31*DATOS!$B$28+'COST PER TASK'!AC31*'COST PER TASK'!AE31*DATOS!$B$29</f>
+        <v>2400</v>
+      </c>
       <c r="AK31" s="8">
         <f t="shared" si="1"/>
-        <v>4363.8584359163142</v>
+        <v>6763.8584359163142</v>
       </c>
       <c r="AL31" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387713</v>
+        <v>225.46194786387713</v>
       </c>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.2">
@@ -3194,21 +3311,25 @@
         <f>AF32*C32*DATOS!$B$3+'COST PER TASK'!AF32*'COST PER TASK'!D32*DATOS!$B$4+'COST PER TASK'!AF32*'COST PER TASK'!E32*DATOS!$B$5</f>
         <v>2628.5714285714284</v>
       </c>
-      <c r="AH32" s="3">
+      <c r="AH32" s="4">
         <f>F32*AE32*DATOS!$D$6+'COST PER TASK'!G32*'COST PER TASK'!AE32*DATOS!$D$7+'COST PER TASK'!H32*'COST PER TASK'!AE32*DATOS!$D$8+'COST PER TASK'!I32*'COST PER TASK'!AE32*DATOS!$D$9+'COST PER TASK'!J32*'COST PER TASK'!AE32*DATOS!$D$10+'COST PER TASK'!K32*'COST PER TASK'!AE32*DATOS!$D$11+'COST PER TASK'!L32*'COST PER TASK'!AE32*DATOS!$D$12+'COST PER TASK'!M32*'COST PER TASK'!AE32*DATOS!$D$13+'COST PER TASK'!N32*'COST PER TASK'!AE32*DATOS!$D$14+'COST PER TASK'!O32*'COST PER TASK'!AE32*DATOS!$D$15</f>
         <v>280.66752870611418</v>
       </c>
-      <c r="AI32" s="3">
+      <c r="AI32" s="4">
         <f>'COST PER TASK'!P32*'COST PER TASK'!AE32*DATOS!$D$16+'COST PER TASK'!Q32*'COST PER TASK'!AE32*DATOS!$D$17+'COST PER TASK'!R32*'COST PER TASK'!AE32*DATOS!$D$18+'COST PER TASK'!S32*'COST PER TASK'!AE32*DATOS!$D$19+'COST PER TASK'!T32*'COST PER TASK'!AE32*DATOS!$D$20+'COST PER TASK'!U32*'COST PER TASK'!AE32*DATOS!$D$21+'COST PER TASK'!V32*'COST PER TASK'!AE32*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ32" s="4">
+        <f>'COST PER TASK'!W32*'COST PER TASK'!AE32*DATOS!$B$23+'COST PER TASK'!X32*'COST PER TASK'!AE32*DATOS!$B$24+'COST PER TASK'!Y32*'COST PER TASK'!AE32*DATOS!$B$25+'COST PER TASK'!Z32*'COST PER TASK'!AE32*DATOS!$B$26+'COST PER TASK'!AA32*'COST PER TASK'!AE32*DATOS!$B$27+'COST PER TASK'!AB32*'COST PER TASK'!AE32*DATOS!$B$28+'COST PER TASK'!AC32*'COST PER TASK'!AE32*DATOS!$B$29</f>
+        <v>1600</v>
+      </c>
       <c r="AK32" s="8">
         <f t="shared" si="1"/>
-        <v>2909.2389572775428</v>
+        <v>4509.2389572775428</v>
       </c>
       <c r="AL32" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387713</v>
+        <v>225.46194786387713</v>
       </c>
     </row>
     <row r="33" spans="2:38" x14ac:dyDescent="0.2">
@@ -3251,21 +3372,25 @@
         <f>AF33*C33*DATOS!$B$3+'COST PER TASK'!AF33*'COST PER TASK'!D33*DATOS!$B$4+'COST PER TASK'!AF33*'COST PER TASK'!E33*DATOS!$B$5</f>
         <v>1520</v>
       </c>
-      <c r="AH33" s="3">
+      <c r="AH33" s="4">
         <f>F33*AE33*DATOS!$D$6+'COST PER TASK'!G33*'COST PER TASK'!AE33*DATOS!$D$7+'COST PER TASK'!H33*'COST PER TASK'!AE33*DATOS!$D$8+'COST PER TASK'!I33*'COST PER TASK'!AE33*DATOS!$D$9+'COST PER TASK'!J33*'COST PER TASK'!AE33*DATOS!$D$10+'COST PER TASK'!K33*'COST PER TASK'!AE33*DATOS!$D$11+'COST PER TASK'!L33*'COST PER TASK'!AE33*DATOS!$D$12+'COST PER TASK'!M33*'COST PER TASK'!AE33*DATOS!$D$13+'COST PER TASK'!N33*'COST PER TASK'!AE33*DATOS!$D$14+'COST PER TASK'!O33*'COST PER TASK'!AE33*DATOS!$D$15</f>
         <v>140.33376435305709</v>
       </c>
-      <c r="AI33" s="3">
+      <c r="AI33" s="4">
         <f>'COST PER TASK'!P33*'COST PER TASK'!AE33*DATOS!$D$16+'COST PER TASK'!Q33*'COST PER TASK'!AE33*DATOS!$D$17+'COST PER TASK'!R33*'COST PER TASK'!AE33*DATOS!$D$18+'COST PER TASK'!S33*'COST PER TASK'!AE33*DATOS!$D$19+'COST PER TASK'!T33*'COST PER TASK'!AE33*DATOS!$D$20+'COST PER TASK'!U33*'COST PER TASK'!AE33*DATOS!$D$21+'COST PER TASK'!V33*'COST PER TASK'!AE33*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ33" s="4">
+        <f>'COST PER TASK'!W33*'COST PER TASK'!AE33*DATOS!$B$23+'COST PER TASK'!X33*'COST PER TASK'!AE33*DATOS!$B$24+'COST PER TASK'!Y33*'COST PER TASK'!AE33*DATOS!$B$25+'COST PER TASK'!Z33*'COST PER TASK'!AE33*DATOS!$B$26+'COST PER TASK'!AA33*'COST PER TASK'!AE33*DATOS!$B$27+'COST PER TASK'!AB33*'COST PER TASK'!AE33*DATOS!$B$28+'COST PER TASK'!AC33*'COST PER TASK'!AE33*DATOS!$B$29</f>
+        <v>400</v>
+      </c>
       <c r="AK33" s="8">
         <f t="shared" si="1"/>
-        <v>1660.3337643530572</v>
+        <v>2060.3337643530572</v>
       </c>
       <c r="AL33" s="8">
         <f t="shared" si="2"/>
-        <v>166.03337643530571</v>
+        <v>206.03337643530571</v>
       </c>
     </row>
     <row r="34" spans="2:38" x14ac:dyDescent="0.2">
@@ -3311,21 +3436,25 @@
         <f>AF34*C34*DATOS!$B$3+'COST PER TASK'!AF34*'COST PER TASK'!D34*DATOS!$B$4+'COST PER TASK'!AF34*'COST PER TASK'!E34*DATOS!$B$5</f>
         <v>2628.5714285714284</v>
       </c>
-      <c r="AH34" s="3">
+      <c r="AH34" s="4">
         <f>F34*AE34*DATOS!$D$6+'COST PER TASK'!G34*'COST PER TASK'!AE34*DATOS!$D$7+'COST PER TASK'!H34*'COST PER TASK'!AE34*DATOS!$D$8+'COST PER TASK'!I34*'COST PER TASK'!AE34*DATOS!$D$9+'COST PER TASK'!J34*'COST PER TASK'!AE34*DATOS!$D$10+'COST PER TASK'!K34*'COST PER TASK'!AE34*DATOS!$D$11+'COST PER TASK'!L34*'COST PER TASK'!AE34*DATOS!$D$12+'COST PER TASK'!M34*'COST PER TASK'!AE34*DATOS!$D$13+'COST PER TASK'!N34*'COST PER TASK'!AE34*DATOS!$D$14+'COST PER TASK'!O34*'COST PER TASK'!AE34*DATOS!$D$15</f>
         <v>70.77988825667596</v>
       </c>
-      <c r="AI34" s="3">
+      <c r="AI34" s="4">
         <f>'COST PER TASK'!P34*'COST PER TASK'!AE34*DATOS!$D$16+'COST PER TASK'!Q34*'COST PER TASK'!AE34*DATOS!$D$17+'COST PER TASK'!R34*'COST PER TASK'!AE34*DATOS!$D$18+'COST PER TASK'!S34*'COST PER TASK'!AE34*DATOS!$D$19+'COST PER TASK'!T34*'COST PER TASK'!AE34*DATOS!$D$20+'COST PER TASK'!U34*'COST PER TASK'!AE34*DATOS!$D$21+'COST PER TASK'!V34*'COST PER TASK'!AE34*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ34" s="4">
+        <f>'COST PER TASK'!W34*'COST PER TASK'!AE34*DATOS!$B$23+'COST PER TASK'!X34*'COST PER TASK'!AE34*DATOS!$B$24+'COST PER TASK'!Y34*'COST PER TASK'!AE34*DATOS!$B$25+'COST PER TASK'!Z34*'COST PER TASK'!AE34*DATOS!$B$26+'COST PER TASK'!AA34*'COST PER TASK'!AE34*DATOS!$B$27+'COST PER TASK'!AB34*'COST PER TASK'!AE34*DATOS!$B$28+'COST PER TASK'!AC34*'COST PER TASK'!AE34*DATOS!$B$29</f>
+        <v>1600</v>
+      </c>
       <c r="AK34" s="8">
         <f t="shared" si="1"/>
-        <v>2699.3513168281042</v>
+        <v>4299.3513168281042</v>
       </c>
       <c r="AL34" s="8">
         <f t="shared" si="2"/>
-        <v>134.96756584140522</v>
+        <v>214.96756584140522</v>
       </c>
     </row>
     <row r="35" spans="2:38" x14ac:dyDescent="0.2">
@@ -3371,21 +3500,25 @@
         <f>AF35*C35*DATOS!$B$3+'COST PER TASK'!AF35*'COST PER TASK'!D35*DATOS!$B$4+'COST PER TASK'!AF35*'COST PER TASK'!E35*DATOS!$B$5</f>
         <v>5257.1428571428569</v>
       </c>
-      <c r="AH35" s="3">
+      <c r="AH35" s="4">
         <f>F35*AE35*DATOS!$D$6+'COST PER TASK'!G35*'COST PER TASK'!AE35*DATOS!$D$7+'COST PER TASK'!H35*'COST PER TASK'!AE35*DATOS!$D$8+'COST PER TASK'!I35*'COST PER TASK'!AE35*DATOS!$D$9+'COST PER TASK'!J35*'COST PER TASK'!AE35*DATOS!$D$10+'COST PER TASK'!K35*'COST PER TASK'!AE35*DATOS!$D$11+'COST PER TASK'!L35*'COST PER TASK'!AE35*DATOS!$D$12+'COST PER TASK'!M35*'COST PER TASK'!AE35*DATOS!$D$13+'COST PER TASK'!N35*'COST PER TASK'!AE35*DATOS!$D$14+'COST PER TASK'!O35*'COST PER TASK'!AE35*DATOS!$D$15</f>
         <v>141.55977651335192</v>
       </c>
-      <c r="AI35" s="3">
+      <c r="AI35" s="4">
         <f>'COST PER TASK'!P35*'COST PER TASK'!AE35*DATOS!$D$16+'COST PER TASK'!Q35*'COST PER TASK'!AE35*DATOS!$D$17+'COST PER TASK'!R35*'COST PER TASK'!AE35*DATOS!$D$18+'COST PER TASK'!S35*'COST PER TASK'!AE35*DATOS!$D$19+'COST PER TASK'!T35*'COST PER TASK'!AE35*DATOS!$D$20+'COST PER TASK'!U35*'COST PER TASK'!AE35*DATOS!$D$21+'COST PER TASK'!V35*'COST PER TASK'!AE35*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ35" s="4">
+        <f>'COST PER TASK'!W35*'COST PER TASK'!AE35*DATOS!$B$23+'COST PER TASK'!X35*'COST PER TASK'!AE35*DATOS!$B$24+'COST PER TASK'!Y35*'COST PER TASK'!AE35*DATOS!$B$25+'COST PER TASK'!Z35*'COST PER TASK'!AE35*DATOS!$B$26+'COST PER TASK'!AA35*'COST PER TASK'!AE35*DATOS!$B$27+'COST PER TASK'!AB35*'COST PER TASK'!AE35*DATOS!$B$28+'COST PER TASK'!AC35*'COST PER TASK'!AE35*DATOS!$B$29</f>
+        <v>3200</v>
+      </c>
       <c r="AK35" s="8">
         <f t="shared" si="1"/>
-        <v>5398.7026336562085</v>
+        <v>8598.7026336562085</v>
       </c>
       <c r="AL35" s="8">
         <f t="shared" si="2"/>
-        <v>134.96756584140522</v>
+        <v>214.96756584140522</v>
       </c>
     </row>
     <row r="36" spans="2:38" x14ac:dyDescent="0.2">
@@ -3431,21 +3564,25 @@
         <f>AF36*C36*DATOS!$B$3+'COST PER TASK'!AF36*'COST PER TASK'!D36*DATOS!$B$4+'COST PER TASK'!AF36*'COST PER TASK'!E36*DATOS!$B$5</f>
         <v>2628.5714285714284</v>
       </c>
-      <c r="AH36" s="3">
+      <c r="AH36" s="4">
         <f>F36*AE36*DATOS!$D$6+'COST PER TASK'!G36*'COST PER TASK'!AE36*DATOS!$D$7+'COST PER TASK'!H36*'COST PER TASK'!AE36*DATOS!$D$8+'COST PER TASK'!I36*'COST PER TASK'!AE36*DATOS!$D$9+'COST PER TASK'!J36*'COST PER TASK'!AE36*DATOS!$D$10+'COST PER TASK'!K36*'COST PER TASK'!AE36*DATOS!$D$11+'COST PER TASK'!L36*'COST PER TASK'!AE36*DATOS!$D$12+'COST PER TASK'!M36*'COST PER TASK'!AE36*DATOS!$D$13+'COST PER TASK'!N36*'COST PER TASK'!AE36*DATOS!$D$14+'COST PER TASK'!O36*'COST PER TASK'!AE36*DATOS!$D$15</f>
         <v>70.77988825667596</v>
       </c>
-      <c r="AI36" s="3">
+      <c r="AI36" s="4">
         <f>'COST PER TASK'!P36*'COST PER TASK'!AE36*DATOS!$D$16+'COST PER TASK'!Q36*'COST PER TASK'!AE36*DATOS!$D$17+'COST PER TASK'!R36*'COST PER TASK'!AE36*DATOS!$D$18+'COST PER TASK'!S36*'COST PER TASK'!AE36*DATOS!$D$19+'COST PER TASK'!T36*'COST PER TASK'!AE36*DATOS!$D$20+'COST PER TASK'!U36*'COST PER TASK'!AE36*DATOS!$D$21+'COST PER TASK'!V36*'COST PER TASK'!AE36*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ36" s="4">
+        <f>'COST PER TASK'!W36*'COST PER TASK'!AE36*DATOS!$B$23+'COST PER TASK'!X36*'COST PER TASK'!AE36*DATOS!$B$24+'COST PER TASK'!Y36*'COST PER TASK'!AE36*DATOS!$B$25+'COST PER TASK'!Z36*'COST PER TASK'!AE36*DATOS!$B$26+'COST PER TASK'!AA36*'COST PER TASK'!AE36*DATOS!$B$27+'COST PER TASK'!AB36*'COST PER TASK'!AE36*DATOS!$B$28+'COST PER TASK'!AC36*'COST PER TASK'!AE36*DATOS!$B$29</f>
+        <v>1600</v>
+      </c>
       <c r="AK36" s="8">
         <f t="shared" si="1"/>
-        <v>2699.3513168281042</v>
+        <v>4299.3513168281042</v>
       </c>
       <c r="AL36" s="8">
         <f t="shared" si="2"/>
-        <v>134.96756584140522</v>
+        <v>214.96756584140522</v>
       </c>
     </row>
     <row r="37" spans="2:38" x14ac:dyDescent="0.2">
@@ -3491,21 +3628,25 @@
         <f>AF37*C37*DATOS!$B$3+'COST PER TASK'!AF37*'COST PER TASK'!D37*DATOS!$B$4+'COST PER TASK'!AF37*'COST PER TASK'!E37*DATOS!$B$5</f>
         <v>26285.71428571429</v>
       </c>
-      <c r="AH37" s="3">
+      <c r="AH37" s="4">
         <f>F37*AE37*DATOS!$D$6+'COST PER TASK'!G37*'COST PER TASK'!AE37*DATOS!$D$7+'COST PER TASK'!H37*'COST PER TASK'!AE37*DATOS!$D$8+'COST PER TASK'!I37*'COST PER TASK'!AE37*DATOS!$D$9+'COST PER TASK'!J37*'COST PER TASK'!AE37*DATOS!$D$10+'COST PER TASK'!K37*'COST PER TASK'!AE37*DATOS!$D$11+'COST PER TASK'!L37*'COST PER TASK'!AE37*DATOS!$D$12+'COST PER TASK'!M37*'COST PER TASK'!AE37*DATOS!$D$13+'COST PER TASK'!N37*'COST PER TASK'!AE37*DATOS!$D$14+'COST PER TASK'!O37*'COST PER TASK'!AE37*DATOS!$D$15</f>
         <v>2806.6752870611417</v>
       </c>
-      <c r="AI37" s="3">
+      <c r="AI37" s="4">
         <f>'COST PER TASK'!P37*'COST PER TASK'!AE37*DATOS!$D$16+'COST PER TASK'!Q37*'COST PER TASK'!AE37*DATOS!$D$17+'COST PER TASK'!R37*'COST PER TASK'!AE37*DATOS!$D$18+'COST PER TASK'!S37*'COST PER TASK'!AE37*DATOS!$D$19+'COST PER TASK'!T37*'COST PER TASK'!AE37*DATOS!$D$20+'COST PER TASK'!U37*'COST PER TASK'!AE37*DATOS!$D$21+'COST PER TASK'!V37*'COST PER TASK'!AE37*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ37" s="4">
+        <f>'COST PER TASK'!W37*'COST PER TASK'!AE37*DATOS!$B$23+'COST PER TASK'!X37*'COST PER TASK'!AE37*DATOS!$B$24+'COST PER TASK'!Y37*'COST PER TASK'!AE37*DATOS!$B$25+'COST PER TASK'!Z37*'COST PER TASK'!AE37*DATOS!$B$26+'COST PER TASK'!AA37*'COST PER TASK'!AE37*DATOS!$B$27+'COST PER TASK'!AB37*'COST PER TASK'!AE37*DATOS!$B$28+'COST PER TASK'!AC37*'COST PER TASK'!AE37*DATOS!$B$29</f>
+        <v>80000</v>
+      </c>
       <c r="AK37" s="8">
         <f t="shared" si="1"/>
-        <v>29092.389572775432</v>
+        <v>109092.38957277543</v>
       </c>
       <c r="AL37" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387716</v>
+        <v>545.46194786387719</v>
       </c>
     </row>
     <row r="38" spans="2:38" x14ac:dyDescent="0.2">
@@ -3551,21 +3692,25 @@
         <f>AF38*C38*DATOS!$B$3+'COST PER TASK'!AF38*'COST PER TASK'!D38*DATOS!$B$4+'COST PER TASK'!AF38*'COST PER TASK'!E38*DATOS!$B$5</f>
         <v>7885.7142857142862</v>
       </c>
-      <c r="AH38" s="3">
+      <c r="AH38" s="4">
         <f>F38*AE38*DATOS!$D$6+'COST PER TASK'!G38*'COST PER TASK'!AE38*DATOS!$D$7+'COST PER TASK'!H38*'COST PER TASK'!AE38*DATOS!$D$8+'COST PER TASK'!I38*'COST PER TASK'!AE38*DATOS!$D$9+'COST PER TASK'!J38*'COST PER TASK'!AE38*DATOS!$D$10+'COST PER TASK'!K38*'COST PER TASK'!AE38*DATOS!$D$11+'COST PER TASK'!L38*'COST PER TASK'!AE38*DATOS!$D$12+'COST PER TASK'!M38*'COST PER TASK'!AE38*DATOS!$D$13+'COST PER TASK'!N38*'COST PER TASK'!AE38*DATOS!$D$14+'COST PER TASK'!O38*'COST PER TASK'!AE38*DATOS!$D$15</f>
         <v>842.00258611834249</v>
       </c>
-      <c r="AI38" s="3">
+      <c r="AI38" s="4">
         <f>'COST PER TASK'!P38*'COST PER TASK'!AE38*DATOS!$D$16+'COST PER TASK'!Q38*'COST PER TASK'!AE38*DATOS!$D$17+'COST PER TASK'!R38*'COST PER TASK'!AE38*DATOS!$D$18+'COST PER TASK'!S38*'COST PER TASK'!AE38*DATOS!$D$19+'COST PER TASK'!T38*'COST PER TASK'!AE38*DATOS!$D$20+'COST PER TASK'!U38*'COST PER TASK'!AE38*DATOS!$D$21+'COST PER TASK'!V38*'COST PER TASK'!AE38*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ38" s="4">
+        <f>'COST PER TASK'!W38*'COST PER TASK'!AE38*DATOS!$B$23+'COST PER TASK'!X38*'COST PER TASK'!AE38*DATOS!$B$24+'COST PER TASK'!Y38*'COST PER TASK'!AE38*DATOS!$B$25+'COST PER TASK'!Z38*'COST PER TASK'!AE38*DATOS!$B$26+'COST PER TASK'!AA38*'COST PER TASK'!AE38*DATOS!$B$27+'COST PER TASK'!AB38*'COST PER TASK'!AE38*DATOS!$B$28+'COST PER TASK'!AC38*'COST PER TASK'!AE38*DATOS!$B$29</f>
+        <v>2400</v>
+      </c>
       <c r="AK38" s="8">
         <f t="shared" si="1"/>
-        <v>8727.7168718326284</v>
+        <v>11127.716871832628</v>
       </c>
       <c r="AL38" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387713</v>
+        <v>185.46194786387713</v>
       </c>
     </row>
     <row r="39" spans="2:38" x14ac:dyDescent="0.2">
@@ -3611,21 +3756,25 @@
         <f>AF39*C39*DATOS!$B$3+'COST PER TASK'!AF39*'COST PER TASK'!D39*DATOS!$B$4+'COST PER TASK'!AF39*'COST PER TASK'!E39*DATOS!$B$5</f>
         <v>26285.71428571429</v>
       </c>
-      <c r="AH39" s="3">
+      <c r="AH39" s="4">
         <f>F39*AE39*DATOS!$D$6+'COST PER TASK'!G39*'COST PER TASK'!AE39*DATOS!$D$7+'COST PER TASK'!H39*'COST PER TASK'!AE39*DATOS!$D$8+'COST PER TASK'!I39*'COST PER TASK'!AE39*DATOS!$D$9+'COST PER TASK'!J39*'COST PER TASK'!AE39*DATOS!$D$10+'COST PER TASK'!K39*'COST PER TASK'!AE39*DATOS!$D$11+'COST PER TASK'!L39*'COST PER TASK'!AE39*DATOS!$D$12+'COST PER TASK'!M39*'COST PER TASK'!AE39*DATOS!$D$13+'COST PER TASK'!N39*'COST PER TASK'!AE39*DATOS!$D$14+'COST PER TASK'!O39*'COST PER TASK'!AE39*DATOS!$D$15</f>
         <v>2806.6752870611417</v>
       </c>
-      <c r="AI39" s="3">
+      <c r="AI39" s="4">
         <f>'COST PER TASK'!P39*'COST PER TASK'!AE39*DATOS!$D$16+'COST PER TASK'!Q39*'COST PER TASK'!AE39*DATOS!$D$17+'COST PER TASK'!R39*'COST PER TASK'!AE39*DATOS!$D$18+'COST PER TASK'!S39*'COST PER TASK'!AE39*DATOS!$D$19+'COST PER TASK'!T39*'COST PER TASK'!AE39*DATOS!$D$20+'COST PER TASK'!U39*'COST PER TASK'!AE39*DATOS!$D$21+'COST PER TASK'!V39*'COST PER TASK'!AE39*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ39" s="4">
+        <f>'COST PER TASK'!W39*'COST PER TASK'!AE39*DATOS!$B$23+'COST PER TASK'!X39*'COST PER TASK'!AE39*DATOS!$B$24+'COST PER TASK'!Y39*'COST PER TASK'!AE39*DATOS!$B$25+'COST PER TASK'!Z39*'COST PER TASK'!AE39*DATOS!$B$26+'COST PER TASK'!AA39*'COST PER TASK'!AE39*DATOS!$B$27+'COST PER TASK'!AB39*'COST PER TASK'!AE39*DATOS!$B$28+'COST PER TASK'!AC39*'COST PER TASK'!AE39*DATOS!$B$29</f>
+        <v>16000</v>
+      </c>
       <c r="AK39" s="8">
         <f t="shared" si="1"/>
-        <v>29092.389572775432</v>
+        <v>45092.389572775428</v>
       </c>
       <c r="AL39" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387716</v>
+        <v>225.46194786387713</v>
       </c>
     </row>
     <row r="40" spans="2:38" x14ac:dyDescent="0.2">
@@ -3671,21 +3820,25 @@
         <f>AF40*C40*DATOS!$B$3+'COST PER TASK'!AF40*'COST PER TASK'!D40*DATOS!$B$4+'COST PER TASK'!AF40*'COST PER TASK'!E40*DATOS!$B$5</f>
         <v>26285.71428571429</v>
       </c>
-      <c r="AH40" s="3">
+      <c r="AH40" s="4">
         <f>F40*AE40*DATOS!$D$6+'COST PER TASK'!G40*'COST PER TASK'!AE40*DATOS!$D$7+'COST PER TASK'!H40*'COST PER TASK'!AE40*DATOS!$D$8+'COST PER TASK'!I40*'COST PER TASK'!AE40*DATOS!$D$9+'COST PER TASK'!J40*'COST PER TASK'!AE40*DATOS!$D$10+'COST PER TASK'!K40*'COST PER TASK'!AE40*DATOS!$D$11+'COST PER TASK'!L40*'COST PER TASK'!AE40*DATOS!$D$12+'COST PER TASK'!M40*'COST PER TASK'!AE40*DATOS!$D$13+'COST PER TASK'!N40*'COST PER TASK'!AE40*DATOS!$D$14+'COST PER TASK'!O40*'COST PER TASK'!AE40*DATOS!$D$15</f>
         <v>2806.6752870611417</v>
       </c>
-      <c r="AI40" s="3">
+      <c r="AI40" s="4">
         <f>'COST PER TASK'!P40*'COST PER TASK'!AE40*DATOS!$D$16+'COST PER TASK'!Q40*'COST PER TASK'!AE40*DATOS!$D$17+'COST PER TASK'!R40*'COST PER TASK'!AE40*DATOS!$D$18+'COST PER TASK'!S40*'COST PER TASK'!AE40*DATOS!$D$19+'COST PER TASK'!T40*'COST PER TASK'!AE40*DATOS!$D$20+'COST PER TASK'!U40*'COST PER TASK'!AE40*DATOS!$D$21+'COST PER TASK'!V40*'COST PER TASK'!AE40*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ40" s="4">
+        <f>'COST PER TASK'!W40*'COST PER TASK'!AE40*DATOS!$B$23+'COST PER TASK'!X40*'COST PER TASK'!AE40*DATOS!$B$24+'COST PER TASK'!Y40*'COST PER TASK'!AE40*DATOS!$B$25+'COST PER TASK'!Z40*'COST PER TASK'!AE40*DATOS!$B$26+'COST PER TASK'!AA40*'COST PER TASK'!AE40*DATOS!$B$27+'COST PER TASK'!AB40*'COST PER TASK'!AE40*DATOS!$B$28+'COST PER TASK'!AC40*'COST PER TASK'!AE40*DATOS!$B$29</f>
+        <v>16000</v>
+      </c>
       <c r="AK40" s="8">
         <f t="shared" si="1"/>
-        <v>29092.389572775432</v>
+        <v>45092.389572775428</v>
       </c>
       <c r="AL40" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387716</v>
+        <v>225.46194786387713</v>
       </c>
     </row>
     <row r="41" spans="2:38" x14ac:dyDescent="0.2">
@@ -3731,21 +3884,25 @@
         <f>AF41*C41*DATOS!$B$3+'COST PER TASK'!AF41*'COST PER TASK'!D41*DATOS!$B$4+'COST PER TASK'!AF41*'COST PER TASK'!E41*DATOS!$B$5</f>
         <v>7885.7142857142862</v>
       </c>
-      <c r="AH41" s="3">
+      <c r="AH41" s="4">
         <f>F41*AE41*DATOS!$D$6+'COST PER TASK'!G41*'COST PER TASK'!AE41*DATOS!$D$7+'COST PER TASK'!H41*'COST PER TASK'!AE41*DATOS!$D$8+'COST PER TASK'!I41*'COST PER TASK'!AE41*DATOS!$D$9+'COST PER TASK'!J41*'COST PER TASK'!AE41*DATOS!$D$10+'COST PER TASK'!K41*'COST PER TASK'!AE41*DATOS!$D$11+'COST PER TASK'!L41*'COST PER TASK'!AE41*DATOS!$D$12+'COST PER TASK'!M41*'COST PER TASK'!AE41*DATOS!$D$13+'COST PER TASK'!N41*'COST PER TASK'!AE41*DATOS!$D$14+'COST PER TASK'!O41*'COST PER TASK'!AE41*DATOS!$D$15</f>
         <v>842.00258611834249</v>
       </c>
-      <c r="AI41" s="3">
+      <c r="AI41" s="4">
         <f>'COST PER TASK'!P41*'COST PER TASK'!AE41*DATOS!$D$16+'COST PER TASK'!Q41*'COST PER TASK'!AE41*DATOS!$D$17+'COST PER TASK'!R41*'COST PER TASK'!AE41*DATOS!$D$18+'COST PER TASK'!S41*'COST PER TASK'!AE41*DATOS!$D$19+'COST PER TASK'!T41*'COST PER TASK'!AE41*DATOS!$D$20+'COST PER TASK'!U41*'COST PER TASK'!AE41*DATOS!$D$21+'COST PER TASK'!V41*'COST PER TASK'!AE41*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ41" s="4">
+        <f>'COST PER TASK'!W41*'COST PER TASK'!AE41*DATOS!$B$23+'COST PER TASK'!X41*'COST PER TASK'!AE41*DATOS!$B$24+'COST PER TASK'!Y41*'COST PER TASK'!AE41*DATOS!$B$25+'COST PER TASK'!Z41*'COST PER TASK'!AE41*DATOS!$B$26+'COST PER TASK'!AA41*'COST PER TASK'!AE41*DATOS!$B$27+'COST PER TASK'!AB41*'COST PER TASK'!AE41*DATOS!$B$28+'COST PER TASK'!AC41*'COST PER TASK'!AE41*DATOS!$B$29</f>
+        <v>2400</v>
+      </c>
       <c r="AK41" s="8">
         <f t="shared" si="1"/>
-        <v>8727.7168718326284</v>
+        <v>11127.716871832628</v>
       </c>
       <c r="AL41" s="8">
         <f t="shared" si="2"/>
-        <v>145.46194786387713</v>
+        <v>185.46194786387713</v>
       </c>
     </row>
     <row r="42" spans="2:38" x14ac:dyDescent="0.2">
@@ -3791,21 +3948,25 @@
         <f>AF42*C42*DATOS!$B$3+'COST PER TASK'!AF42*'COST PER TASK'!D42*DATOS!$B$4+'COST PER TASK'!AF42*'COST PER TASK'!E42*DATOS!$B$5</f>
         <v>13142.857142857145</v>
       </c>
-      <c r="AH42" s="3">
+      <c r="AH42" s="4">
         <f>F42*AE42*DATOS!$D$6+'COST PER TASK'!G42*'COST PER TASK'!AE42*DATOS!$D$7+'COST PER TASK'!H42*'COST PER TASK'!AE42*DATOS!$D$8+'COST PER TASK'!I42*'COST PER TASK'!AE42*DATOS!$D$9+'COST PER TASK'!J42*'COST PER TASK'!AE42*DATOS!$D$10+'COST PER TASK'!K42*'COST PER TASK'!AE42*DATOS!$D$11+'COST PER TASK'!L42*'COST PER TASK'!AE42*DATOS!$D$12+'COST PER TASK'!M42*'COST PER TASK'!AE42*DATOS!$D$13+'COST PER TASK'!N42*'COST PER TASK'!AE42*DATOS!$D$14+'COST PER TASK'!O42*'COST PER TASK'!AE42*DATOS!$D$15</f>
         <v>353.89944128337982</v>
       </c>
-      <c r="AI42" s="3">
+      <c r="AI42" s="4">
         <f>'COST PER TASK'!P42*'COST PER TASK'!AE42*DATOS!$D$16+'COST PER TASK'!Q42*'COST PER TASK'!AE42*DATOS!$D$17+'COST PER TASK'!R42*'COST PER TASK'!AE42*DATOS!$D$18+'COST PER TASK'!S42*'COST PER TASK'!AE42*DATOS!$D$19+'COST PER TASK'!T42*'COST PER TASK'!AE42*DATOS!$D$20+'COST PER TASK'!U42*'COST PER TASK'!AE42*DATOS!$D$21+'COST PER TASK'!V42*'COST PER TASK'!AE42*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ42" s="4">
+        <f>'COST PER TASK'!W42*'COST PER TASK'!AE42*DATOS!$B$23+'COST PER TASK'!X42*'COST PER TASK'!AE42*DATOS!$B$24+'COST PER TASK'!Y42*'COST PER TASK'!AE42*DATOS!$B$25+'COST PER TASK'!Z42*'COST PER TASK'!AE42*DATOS!$B$26+'COST PER TASK'!AA42*'COST PER TASK'!AE42*DATOS!$B$27+'COST PER TASK'!AB42*'COST PER TASK'!AE42*DATOS!$B$28+'COST PER TASK'!AC42*'COST PER TASK'!AE42*DATOS!$B$29</f>
+        <v>8000</v>
+      </c>
       <c r="AK42" s="8">
         <f t="shared" si="1"/>
-        <v>13496.756584140525</v>
+        <v>21496.756584140523</v>
       </c>
       <c r="AL42" s="8">
         <f t="shared" si="2"/>
-        <v>134.96756584140525</v>
+        <v>214.96756584140522</v>
       </c>
     </row>
     <row r="43" spans="2:38" x14ac:dyDescent="0.2">
@@ -3851,21 +4012,25 @@
         <f>AF43*C43*DATOS!$B$3+'COST PER TASK'!AF43*'COST PER TASK'!D43*DATOS!$B$4+'COST PER TASK'!AF43*'COST PER TASK'!E43*DATOS!$B$5</f>
         <v>23657.142857142855</v>
       </c>
-      <c r="AH43" s="3">
+      <c r="AH43" s="4">
         <f>F43*AE43*DATOS!$D$6+'COST PER TASK'!G43*'COST PER TASK'!AE43*DATOS!$D$7+'COST PER TASK'!H43*'COST PER TASK'!AE43*DATOS!$D$8+'COST PER TASK'!I43*'COST PER TASK'!AE43*DATOS!$D$9+'COST PER TASK'!J43*'COST PER TASK'!AE43*DATOS!$D$10+'COST PER TASK'!K43*'COST PER TASK'!AE43*DATOS!$D$11+'COST PER TASK'!L43*'COST PER TASK'!AE43*DATOS!$D$12+'COST PER TASK'!M43*'COST PER TASK'!AE43*DATOS!$D$13+'COST PER TASK'!N43*'COST PER TASK'!AE43*DATOS!$D$14+'COST PER TASK'!O43*'COST PER TASK'!AE43*DATOS!$D$15</f>
         <v>637.01899431008371</v>
       </c>
-      <c r="AI43" s="3">
+      <c r="AI43" s="4">
         <f>'COST PER TASK'!P43*'COST PER TASK'!AE43*DATOS!$D$16+'COST PER TASK'!Q43*'COST PER TASK'!AE43*DATOS!$D$17+'COST PER TASK'!R43*'COST PER TASK'!AE43*DATOS!$D$18+'COST PER TASK'!S43*'COST PER TASK'!AE43*DATOS!$D$19+'COST PER TASK'!T43*'COST PER TASK'!AE43*DATOS!$D$20+'COST PER TASK'!U43*'COST PER TASK'!AE43*DATOS!$D$21+'COST PER TASK'!V43*'COST PER TASK'!AE43*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ43" s="4">
+        <f>'COST PER TASK'!W43*'COST PER TASK'!AE43*DATOS!$B$23+'COST PER TASK'!X43*'COST PER TASK'!AE43*DATOS!$B$24+'COST PER TASK'!Y43*'COST PER TASK'!AE43*DATOS!$B$25+'COST PER TASK'!Z43*'COST PER TASK'!AE43*DATOS!$B$26+'COST PER TASK'!AA43*'COST PER TASK'!AE43*DATOS!$B$27+'COST PER TASK'!AB43*'COST PER TASK'!AE43*DATOS!$B$28+'COST PER TASK'!AC43*'COST PER TASK'!AE43*DATOS!$B$29</f>
+        <v>14400</v>
+      </c>
       <c r="AK43" s="8">
         <f t="shared" si="1"/>
-        <v>24294.16185145294</v>
+        <v>38694.16185145294</v>
       </c>
       <c r="AL43" s="8">
         <f t="shared" si="2"/>
-        <v>134.96756584140522</v>
+        <v>214.96756584140522</v>
       </c>
     </row>
     <row r="44" spans="2:38" x14ac:dyDescent="0.2">
@@ -3911,21 +4076,25 @@
         <f>AF44*C44*DATOS!$B$3+'COST PER TASK'!AF44*'COST PER TASK'!D44*DATOS!$B$4+'COST PER TASK'!AF44*'COST PER TASK'!E44*DATOS!$B$5</f>
         <v>17742.857142857141</v>
       </c>
-      <c r="AH44" s="3">
+      <c r="AH44" s="4">
         <f>F44*AE44*DATOS!$D$6+'COST PER TASK'!G44*'COST PER TASK'!AE44*DATOS!$D$7+'COST PER TASK'!H44*'COST PER TASK'!AE44*DATOS!$D$8+'COST PER TASK'!I44*'COST PER TASK'!AE44*DATOS!$D$9+'COST PER TASK'!J44*'COST PER TASK'!AE44*DATOS!$D$10+'COST PER TASK'!K44*'COST PER TASK'!AE44*DATOS!$D$11+'COST PER TASK'!L44*'COST PER TASK'!AE44*DATOS!$D$12+'COST PER TASK'!M44*'COST PER TASK'!AE44*DATOS!$D$13+'COST PER TASK'!N44*'COST PER TASK'!AE44*DATOS!$D$14+'COST PER TASK'!O44*'COST PER TASK'!AE44*DATOS!$D$15</f>
         <v>477.76424573256276</v>
       </c>
-      <c r="AI44" s="3">
+      <c r="AI44" s="4">
         <f>'COST PER TASK'!P44*'COST PER TASK'!AE44*DATOS!$D$16+'COST PER TASK'!Q44*'COST PER TASK'!AE44*DATOS!$D$17+'COST PER TASK'!R44*'COST PER TASK'!AE44*DATOS!$D$18+'COST PER TASK'!S44*'COST PER TASK'!AE44*DATOS!$D$19+'COST PER TASK'!T44*'COST PER TASK'!AE44*DATOS!$D$20+'COST PER TASK'!U44*'COST PER TASK'!AE44*DATOS!$D$21+'COST PER TASK'!V44*'COST PER TASK'!AE44*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ44" s="4">
+        <f>'COST PER TASK'!W44*'COST PER TASK'!AE44*DATOS!$B$23+'COST PER TASK'!X44*'COST PER TASK'!AE44*DATOS!$B$24+'COST PER TASK'!Y44*'COST PER TASK'!AE44*DATOS!$B$25+'COST PER TASK'!Z44*'COST PER TASK'!AE44*DATOS!$B$26+'COST PER TASK'!AA44*'COST PER TASK'!AE44*DATOS!$B$27+'COST PER TASK'!AB44*'COST PER TASK'!AE44*DATOS!$B$28+'COST PER TASK'!AC44*'COST PER TASK'!AE44*DATOS!$B$29</f>
+        <v>10800</v>
+      </c>
       <c r="AK44" s="8">
         <f t="shared" si="1"/>
-        <v>18220.621388589705</v>
+        <v>29020.621388589705</v>
       </c>
       <c r="AL44" s="8">
         <f t="shared" si="2"/>
-        <v>134.96756584140522</v>
+        <v>214.96756584140522</v>
       </c>
     </row>
     <row r="45" spans="2:38" x14ac:dyDescent="0.2">
@@ -3971,21 +4140,25 @@
         <f>AF45*C45*DATOS!$B$3+'COST PER TASK'!AF45*'COST PER TASK'!D45*DATOS!$B$4+'COST PER TASK'!AF45*'COST PER TASK'!E45*DATOS!$B$5</f>
         <v>3285.7142857142862</v>
       </c>
-      <c r="AH45" s="3">
+      <c r="AH45" s="4">
         <f>F45*AE45*DATOS!$D$6+'COST PER TASK'!G45*'COST PER TASK'!AE45*DATOS!$D$7+'COST PER TASK'!H45*'COST PER TASK'!AE45*DATOS!$D$8+'COST PER TASK'!I45*'COST PER TASK'!AE45*DATOS!$D$9+'COST PER TASK'!J45*'COST PER TASK'!AE45*DATOS!$D$10+'COST PER TASK'!K45*'COST PER TASK'!AE45*DATOS!$D$11+'COST PER TASK'!L45*'COST PER TASK'!AE45*DATOS!$D$12+'COST PER TASK'!M45*'COST PER TASK'!AE45*DATOS!$D$13+'COST PER TASK'!N45*'COST PER TASK'!AE45*DATOS!$D$14+'COST PER TASK'!O45*'COST PER TASK'!AE45*DATOS!$D$15</f>
         <v>88.474860320844954</v>
       </c>
-      <c r="AI45" s="3">
+      <c r="AI45" s="4">
         <f>'COST PER TASK'!P45*'COST PER TASK'!AE45*DATOS!$D$16+'COST PER TASK'!Q45*'COST PER TASK'!AE45*DATOS!$D$17+'COST PER TASK'!R45*'COST PER TASK'!AE45*DATOS!$D$18+'COST PER TASK'!S45*'COST PER TASK'!AE45*DATOS!$D$19+'COST PER TASK'!T45*'COST PER TASK'!AE45*DATOS!$D$20+'COST PER TASK'!U45*'COST PER TASK'!AE45*DATOS!$D$21+'COST PER TASK'!V45*'COST PER TASK'!AE45*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ45" s="4">
+        <f>'COST PER TASK'!W45*'COST PER TASK'!AE45*DATOS!$B$23+'COST PER TASK'!X45*'COST PER TASK'!AE45*DATOS!$B$24+'COST PER TASK'!Y45*'COST PER TASK'!AE45*DATOS!$B$25+'COST PER TASK'!Z45*'COST PER TASK'!AE45*DATOS!$B$26+'COST PER TASK'!AA45*'COST PER TASK'!AE45*DATOS!$B$27+'COST PER TASK'!AB45*'COST PER TASK'!AE45*DATOS!$B$28+'COST PER TASK'!AC45*'COST PER TASK'!AE45*DATOS!$B$29</f>
+        <v>1000</v>
+      </c>
       <c r="AK45" s="8">
         <f t="shared" si="1"/>
-        <v>3374.1891460351312</v>
+        <v>4374.1891460351308</v>
       </c>
       <c r="AL45" s="8">
         <f t="shared" si="2"/>
-        <v>134.96756584140525</v>
+        <v>174.96756584140522</v>
       </c>
     </row>
     <row r="46" spans="2:38" x14ac:dyDescent="0.2">
@@ -4019,21 +4192,25 @@
         <f>AF46*C46*DATOS!$B$3+'COST PER TASK'!AF46*'COST PER TASK'!D46*DATOS!$B$4+'COST PER TASK'!AF46*'COST PER TASK'!E46*DATOS!$B$5</f>
         <v>22400</v>
       </c>
-      <c r="AH46" s="3">
+      <c r="AH46" s="4">
         <f>F46*AE46*DATOS!$D$6+'COST PER TASK'!G46*'COST PER TASK'!AE46*DATOS!$D$7+'COST PER TASK'!H46*'COST PER TASK'!AE46*DATOS!$D$8+'COST PER TASK'!I46*'COST PER TASK'!AE46*DATOS!$D$9+'COST PER TASK'!J46*'COST PER TASK'!AE46*DATOS!$D$10+'COST PER TASK'!K46*'COST PER TASK'!AE46*DATOS!$D$11+'COST PER TASK'!L46*'COST PER TASK'!AE46*DATOS!$D$12+'COST PER TASK'!M46*'COST PER TASK'!AE46*DATOS!$D$13+'COST PER TASK'!N46*'COST PER TASK'!AE46*DATOS!$D$14+'COST PER TASK'!O46*'COST PER TASK'!AE46*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI46" s="3">
+      <c r="AI46" s="4">
         <f>'COST PER TASK'!P46*'COST PER TASK'!AE46*DATOS!$D$16+'COST PER TASK'!Q46*'COST PER TASK'!AE46*DATOS!$D$17+'COST PER TASK'!R46*'COST PER TASK'!AE46*DATOS!$D$18+'COST PER TASK'!S46*'COST PER TASK'!AE46*DATOS!$D$19+'COST PER TASK'!T46*'COST PER TASK'!AE46*DATOS!$D$20+'COST PER TASK'!U46*'COST PER TASK'!AE46*DATOS!$D$21+'COST PER TASK'!V46*'COST PER TASK'!AE46*DATOS!$D$22</f>
         <v>87500</v>
       </c>
+      <c r="AJ46" s="4">
+        <f>'COST PER TASK'!W46*'COST PER TASK'!AE46*DATOS!$B$23+'COST PER TASK'!X46*'COST PER TASK'!AE46*DATOS!$B$24+'COST PER TASK'!Y46*'COST PER TASK'!AE46*DATOS!$B$25+'COST PER TASK'!Z46*'COST PER TASK'!AE46*DATOS!$B$26+'COST PER TASK'!AA46*'COST PER TASK'!AE46*DATOS!$B$27+'COST PER TASK'!AB46*'COST PER TASK'!AE46*DATOS!$B$28+'COST PER TASK'!AC46*'COST PER TASK'!AE46*DATOS!$B$29</f>
+        <v>16000</v>
+      </c>
       <c r="AK46" s="8">
         <f t="shared" si="1"/>
-        <v>109900</v>
+        <v>125900</v>
       </c>
       <c r="AL46" s="8">
         <f t="shared" si="2"/>
-        <v>549.5</v>
+        <v>629.5</v>
       </c>
     </row>
     <row r="47" spans="2:38" x14ac:dyDescent="0.2">
@@ -4076,21 +4253,25 @@
         <f>AF47*C47*DATOS!$B$3+'COST PER TASK'!AF47*'COST PER TASK'!D47*DATOS!$B$4+'COST PER TASK'!AF47*'COST PER TASK'!E47*DATOS!$B$5</f>
         <v>16800</v>
       </c>
-      <c r="AH47" s="3">
+      <c r="AH47" s="4">
         <f>F47*AE47*DATOS!$D$6+'COST PER TASK'!G47*'COST PER TASK'!AE47*DATOS!$D$7+'COST PER TASK'!H47*'COST PER TASK'!AE47*DATOS!$D$8+'COST PER TASK'!I47*'COST PER TASK'!AE47*DATOS!$D$9+'COST PER TASK'!J47*'COST PER TASK'!AE47*DATOS!$D$10+'COST PER TASK'!K47*'COST PER TASK'!AE47*DATOS!$D$11+'COST PER TASK'!L47*'COST PER TASK'!AE47*DATOS!$D$12+'COST PER TASK'!M47*'COST PER TASK'!AE47*DATOS!$D$13+'COST PER TASK'!N47*'COST PER TASK'!AE47*DATOS!$D$14+'COST PER TASK'!O47*'COST PER TASK'!AE47*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI47" s="3">
+      <c r="AI47" s="4">
         <f>'COST PER TASK'!P47*'COST PER TASK'!AE47*DATOS!$D$16+'COST PER TASK'!Q47*'COST PER TASK'!AE47*DATOS!$D$17+'COST PER TASK'!R47*'COST PER TASK'!AE47*DATOS!$D$18+'COST PER TASK'!S47*'COST PER TASK'!AE47*DATOS!$D$19+'COST PER TASK'!T47*'COST PER TASK'!AE47*DATOS!$D$20+'COST PER TASK'!U47*'COST PER TASK'!AE47*DATOS!$D$21+'COST PER TASK'!V47*'COST PER TASK'!AE47*DATOS!$D$22</f>
         <v>94285.71428571429</v>
       </c>
+      <c r="AJ47" s="4">
+        <f>'COST PER TASK'!W47*'COST PER TASK'!AE47*DATOS!$B$23+'COST PER TASK'!X47*'COST PER TASK'!AE47*DATOS!$B$24+'COST PER TASK'!Y47*'COST PER TASK'!AE47*DATOS!$B$25+'COST PER TASK'!Z47*'COST PER TASK'!AE47*DATOS!$B$26+'COST PER TASK'!AA47*'COST PER TASK'!AE47*DATOS!$B$27+'COST PER TASK'!AB47*'COST PER TASK'!AE47*DATOS!$B$28+'COST PER TASK'!AC47*'COST PER TASK'!AE47*DATOS!$B$29</f>
+        <v>12000</v>
+      </c>
       <c r="AK47" s="8">
         <f t="shared" si="1"/>
-        <v>111085.71428571429</v>
+        <v>123085.71428571429</v>
       </c>
       <c r="AL47" s="8">
         <f t="shared" si="2"/>
-        <v>740.57142857142856</v>
+        <v>820.57142857142856</v>
       </c>
     </row>
     <row r="48" spans="2:38" x14ac:dyDescent="0.2">
@@ -4127,21 +4308,25 @@
         <f>AF48*C48*DATOS!$B$3+'COST PER TASK'!AF48*'COST PER TASK'!D48*DATOS!$B$4+'COST PER TASK'!AF48*'COST PER TASK'!E48*DATOS!$B$5</f>
         <v>11200</v>
       </c>
-      <c r="AH48" s="3">
+      <c r="AH48" s="4">
         <f>F48*AE48*DATOS!$D$6+'COST PER TASK'!G48*'COST PER TASK'!AE48*DATOS!$D$7+'COST PER TASK'!H48*'COST PER TASK'!AE48*DATOS!$D$8+'COST PER TASK'!I48*'COST PER TASK'!AE48*DATOS!$D$9+'COST PER TASK'!J48*'COST PER TASK'!AE48*DATOS!$D$10+'COST PER TASK'!K48*'COST PER TASK'!AE48*DATOS!$D$11+'COST PER TASK'!L48*'COST PER TASK'!AE48*DATOS!$D$12+'COST PER TASK'!M48*'COST PER TASK'!AE48*DATOS!$D$13+'COST PER TASK'!N48*'COST PER TASK'!AE48*DATOS!$D$14+'COST PER TASK'!O48*'COST PER TASK'!AE48*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI48" s="3">
+      <c r="AI48" s="4">
         <f>'COST PER TASK'!P48*'COST PER TASK'!AE48*DATOS!$D$16+'COST PER TASK'!Q48*'COST PER TASK'!AE48*DATOS!$D$17+'COST PER TASK'!R48*'COST PER TASK'!AE48*DATOS!$D$18+'COST PER TASK'!S48*'COST PER TASK'!AE48*DATOS!$D$19+'COST PER TASK'!T48*'COST PER TASK'!AE48*DATOS!$D$20+'COST PER TASK'!U48*'COST PER TASK'!AE48*DATOS!$D$21+'COST PER TASK'!V48*'COST PER TASK'!AE48*DATOS!$D$22</f>
         <v>22807.017543859649</v>
       </c>
+      <c r="AJ48" s="4">
+        <f>'COST PER TASK'!W48*'COST PER TASK'!AE48*DATOS!$B$23+'COST PER TASK'!X48*'COST PER TASK'!AE48*DATOS!$B$24+'COST PER TASK'!Y48*'COST PER TASK'!AE48*DATOS!$B$25+'COST PER TASK'!Z48*'COST PER TASK'!AE48*DATOS!$B$26+'COST PER TASK'!AA48*'COST PER TASK'!AE48*DATOS!$B$27+'COST PER TASK'!AB48*'COST PER TASK'!AE48*DATOS!$B$28+'COST PER TASK'!AC48*'COST PER TASK'!AE48*DATOS!$B$29</f>
+        <v>8000</v>
+      </c>
       <c r="AK48" s="8">
         <f t="shared" si="1"/>
-        <v>34007.017543859649</v>
+        <v>42007.017543859649</v>
       </c>
       <c r="AL48" s="8">
         <f t="shared" si="2"/>
-        <v>340.07017543859649</v>
+        <v>420.07017543859649</v>
       </c>
     </row>
     <row r="49" spans="2:38" x14ac:dyDescent="0.2">
@@ -4175,21 +4360,25 @@
         <f>AF49*C49*DATOS!$B$3+'COST PER TASK'!AF49*'COST PER TASK'!D49*DATOS!$B$4+'COST PER TASK'!AF49*'COST PER TASK'!E49*DATOS!$B$5</f>
         <v>6960</v>
       </c>
-      <c r="AH49" s="3">
+      <c r="AH49" s="4">
         <f>F49*AE49*DATOS!$D$6+'COST PER TASK'!G49*'COST PER TASK'!AE49*DATOS!$D$7+'COST PER TASK'!H49*'COST PER TASK'!AE49*DATOS!$D$8+'COST PER TASK'!I49*'COST PER TASK'!AE49*DATOS!$D$9+'COST PER TASK'!J49*'COST PER TASK'!AE49*DATOS!$D$10+'COST PER TASK'!K49*'COST PER TASK'!AE49*DATOS!$D$11+'COST PER TASK'!L49*'COST PER TASK'!AE49*DATOS!$D$12+'COST PER TASK'!M49*'COST PER TASK'!AE49*DATOS!$D$13+'COST PER TASK'!N49*'COST PER TASK'!AE49*DATOS!$D$14+'COST PER TASK'!O49*'COST PER TASK'!AE49*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI49" s="3">
+      <c r="AI49" s="4">
         <f>'COST PER TASK'!P49*'COST PER TASK'!AE49*DATOS!$D$16+'COST PER TASK'!Q49*'COST PER TASK'!AE49*DATOS!$D$17+'COST PER TASK'!R49*'COST PER TASK'!AE49*DATOS!$D$18+'COST PER TASK'!S49*'COST PER TASK'!AE49*DATOS!$D$19+'COST PER TASK'!T49*'COST PER TASK'!AE49*DATOS!$D$20+'COST PER TASK'!U49*'COST PER TASK'!AE49*DATOS!$D$21+'COST PER TASK'!V49*'COST PER TASK'!AE49*DATOS!$D$22</f>
         <v>26250</v>
       </c>
+      <c r="AJ49" s="4">
+        <f>'COST PER TASK'!W49*'COST PER TASK'!AE49*DATOS!$B$23+'COST PER TASK'!X49*'COST PER TASK'!AE49*DATOS!$B$24+'COST PER TASK'!Y49*'COST PER TASK'!AE49*DATOS!$B$25+'COST PER TASK'!Z49*'COST PER TASK'!AE49*DATOS!$B$26+'COST PER TASK'!AA49*'COST PER TASK'!AE49*DATOS!$B$27+'COST PER TASK'!AB49*'COST PER TASK'!AE49*DATOS!$B$28+'COST PER TASK'!AC49*'COST PER TASK'!AE49*DATOS!$B$29</f>
+        <v>28800</v>
+      </c>
       <c r="AK49" s="8">
         <f t="shared" si="1"/>
-        <v>33210</v>
+        <v>62010</v>
       </c>
       <c r="AL49" s="8">
         <f t="shared" si="2"/>
-        <v>553.5</v>
+        <v>1033.5</v>
       </c>
     </row>
     <row r="50" spans="2:38" x14ac:dyDescent="0.2">
@@ -4232,21 +4421,25 @@
         <f>AF50*C50*DATOS!$B$3+'COST PER TASK'!AF50*'COST PER TASK'!D50*DATOS!$B$4+'COST PER TASK'!AF50*'COST PER TASK'!E50*DATOS!$B$5</f>
         <v>6960</v>
       </c>
-      <c r="AH50" s="3">
+      <c r="AH50" s="4">
         <f>F50*AE50*DATOS!$D$6+'COST PER TASK'!G50*'COST PER TASK'!AE50*DATOS!$D$7+'COST PER TASK'!H50*'COST PER TASK'!AE50*DATOS!$D$8+'COST PER TASK'!I50*'COST PER TASK'!AE50*DATOS!$D$9+'COST PER TASK'!J50*'COST PER TASK'!AE50*DATOS!$D$10+'COST PER TASK'!K50*'COST PER TASK'!AE50*DATOS!$D$11+'COST PER TASK'!L50*'COST PER TASK'!AE50*DATOS!$D$12+'COST PER TASK'!M50*'COST PER TASK'!AE50*DATOS!$D$13+'COST PER TASK'!N50*'COST PER TASK'!AE50*DATOS!$D$14+'COST PER TASK'!O50*'COST PER TASK'!AE50*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI50" s="3">
+      <c r="AI50" s="4">
         <f>'COST PER TASK'!P50*'COST PER TASK'!AE50*DATOS!$D$16+'COST PER TASK'!Q50*'COST PER TASK'!AE50*DATOS!$D$17+'COST PER TASK'!R50*'COST PER TASK'!AE50*DATOS!$D$18+'COST PER TASK'!S50*'COST PER TASK'!AE50*DATOS!$D$19+'COST PER TASK'!T50*'COST PER TASK'!AE50*DATOS!$D$20+'COST PER TASK'!U50*'COST PER TASK'!AE50*DATOS!$D$21+'COST PER TASK'!V50*'COST PER TASK'!AE50*DATOS!$D$22</f>
         <v>37714.285714285717</v>
       </c>
+      <c r="AJ50" s="4">
+        <f>'COST PER TASK'!W50*'COST PER TASK'!AE50*DATOS!$B$23+'COST PER TASK'!X50*'COST PER TASK'!AE50*DATOS!$B$24+'COST PER TASK'!Y50*'COST PER TASK'!AE50*DATOS!$B$25+'COST PER TASK'!Z50*'COST PER TASK'!AE50*DATOS!$B$26+'COST PER TASK'!AA50*'COST PER TASK'!AE50*DATOS!$B$27+'COST PER TASK'!AB50*'COST PER TASK'!AE50*DATOS!$B$28+'COST PER TASK'!AC50*'COST PER TASK'!AE50*DATOS!$B$29</f>
+        <v>5760</v>
+      </c>
       <c r="AK50" s="8">
         <f t="shared" si="1"/>
-        <v>44674.285714285717</v>
+        <v>50434.285714285717</v>
       </c>
       <c r="AL50" s="8">
         <f t="shared" si="2"/>
-        <v>744.57142857142867</v>
+        <v>840.57142857142867</v>
       </c>
     </row>
     <row r="51" spans="2:38" x14ac:dyDescent="0.2">
@@ -4280,21 +4473,25 @@
         <f>AF51*C51*DATOS!$B$3+'COST PER TASK'!AF51*'COST PER TASK'!D51*DATOS!$B$4+'COST PER TASK'!AF51*'COST PER TASK'!E51*DATOS!$B$5</f>
         <v>5760</v>
       </c>
-      <c r="AH51" s="3">
+      <c r="AH51" s="4">
         <f>F51*AE51*DATOS!$D$6+'COST PER TASK'!G51*'COST PER TASK'!AE51*DATOS!$D$7+'COST PER TASK'!H51*'COST PER TASK'!AE51*DATOS!$D$8+'COST PER TASK'!I51*'COST PER TASK'!AE51*DATOS!$D$9+'COST PER TASK'!J51*'COST PER TASK'!AE51*DATOS!$D$10+'COST PER TASK'!K51*'COST PER TASK'!AE51*DATOS!$D$11+'COST PER TASK'!L51*'COST PER TASK'!AE51*DATOS!$D$12+'COST PER TASK'!M51*'COST PER TASK'!AE51*DATOS!$D$13+'COST PER TASK'!N51*'COST PER TASK'!AE51*DATOS!$D$14+'COST PER TASK'!O51*'COST PER TASK'!AE51*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI51" s="3">
+      <c r="AI51" s="4">
         <f>'COST PER TASK'!P51*'COST PER TASK'!AE51*DATOS!$D$16+'COST PER TASK'!Q51*'COST PER TASK'!AE51*DATOS!$D$17+'COST PER TASK'!R51*'COST PER TASK'!AE51*DATOS!$D$18+'COST PER TASK'!S51*'COST PER TASK'!AE51*DATOS!$D$19+'COST PER TASK'!T51*'COST PER TASK'!AE51*DATOS!$D$20+'COST PER TASK'!U51*'COST PER TASK'!AE51*DATOS!$D$21+'COST PER TASK'!V51*'COST PER TASK'!AE51*DATOS!$D$22</f>
         <v>10263.157894736843</v>
       </c>
+      <c r="AJ51" s="4">
+        <f>'COST PER TASK'!W51*'COST PER TASK'!AE51*DATOS!$B$23+'COST PER TASK'!X51*'COST PER TASK'!AE51*DATOS!$B$24+'COST PER TASK'!Y51*'COST PER TASK'!AE51*DATOS!$B$25+'COST PER TASK'!Z51*'COST PER TASK'!AE51*DATOS!$B$26+'COST PER TASK'!AA51*'COST PER TASK'!AE51*DATOS!$B$27+'COST PER TASK'!AB51*'COST PER TASK'!AE51*DATOS!$B$28+'COST PER TASK'!AC51*'COST PER TASK'!AE51*DATOS!$B$29</f>
+        <v>4320</v>
+      </c>
       <c r="AK51" s="8">
         <f t="shared" si="1"/>
-        <v>16023.157894736843</v>
+        <v>20343.157894736843</v>
       </c>
       <c r="AL51" s="8">
         <f t="shared" si="2"/>
-        <v>356.07017543859649</v>
+        <v>452.07017543859649</v>
       </c>
     </row>
     <row r="52" spans="2:38" x14ac:dyDescent="0.2">
@@ -4343,21 +4540,25 @@
         <f>AF52*C52*DATOS!$B$3+'COST PER TASK'!AF52*'COST PER TASK'!D52*DATOS!$B$4+'COST PER TASK'!AF52*'COST PER TASK'!E52*DATOS!$B$5</f>
         <v>10240</v>
       </c>
-      <c r="AH52" s="3">
+      <c r="AH52" s="4">
         <f>F52*AE52*DATOS!$D$6+'COST PER TASK'!G52*'COST PER TASK'!AE52*DATOS!$D$7+'COST PER TASK'!H52*'COST PER TASK'!AE52*DATOS!$D$8+'COST PER TASK'!I52*'COST PER TASK'!AE52*DATOS!$D$9+'COST PER TASK'!J52*'COST PER TASK'!AE52*DATOS!$D$10+'COST PER TASK'!K52*'COST PER TASK'!AE52*DATOS!$D$11+'COST PER TASK'!L52*'COST PER TASK'!AE52*DATOS!$D$12+'COST PER TASK'!M52*'COST PER TASK'!AE52*DATOS!$D$13+'COST PER TASK'!N52*'COST PER TASK'!AE52*DATOS!$D$14+'COST PER TASK'!O52*'COST PER TASK'!AE52*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI52" s="3">
+      <c r="AI52" s="4">
         <f>'COST PER TASK'!P52*'COST PER TASK'!AE52*DATOS!$D$16+'COST PER TASK'!Q52*'COST PER TASK'!AE52*DATOS!$D$17+'COST PER TASK'!R52*'COST PER TASK'!AE52*DATOS!$D$18+'COST PER TASK'!S52*'COST PER TASK'!AE52*DATOS!$D$19+'COST PER TASK'!T52*'COST PER TASK'!AE52*DATOS!$D$20+'COST PER TASK'!U52*'COST PER TASK'!AE52*DATOS!$D$21+'COST PER TASK'!V52*'COST PER TASK'!AE52*DATOS!$D$22</f>
         <v>103531.32832080201</v>
       </c>
+      <c r="AJ52" s="4">
+        <f>'COST PER TASK'!W52*'COST PER TASK'!AE52*DATOS!$B$23+'COST PER TASK'!X52*'COST PER TASK'!AE52*DATOS!$B$24+'COST PER TASK'!Y52*'COST PER TASK'!AE52*DATOS!$B$25+'COST PER TASK'!Z52*'COST PER TASK'!AE52*DATOS!$B$26+'COST PER TASK'!AA52*'COST PER TASK'!AE52*DATOS!$B$27+'COST PER TASK'!AB52*'COST PER TASK'!AE52*DATOS!$B$28+'COST PER TASK'!AC52*'COST PER TASK'!AE52*DATOS!$B$29</f>
+        <v>7680</v>
+      </c>
       <c r="AK52" s="8">
         <f t="shared" si="1"/>
-        <v>113771.32832080201</v>
+        <v>121451.32832080201</v>
       </c>
       <c r="AL52" s="8">
         <f t="shared" si="2"/>
-        <v>1422.1416040100253</v>
+        <v>1518.1416040100253</v>
       </c>
     </row>
     <row r="53" spans="2:38" x14ac:dyDescent="0.2">
@@ -4409,21 +4610,25 @@
         <f>AF53*C53*DATOS!$B$3+'COST PER TASK'!AF53*'COST PER TASK'!D53*DATOS!$B$4+'COST PER TASK'!AF53*'COST PER TASK'!E53*DATOS!$B$5</f>
         <v>9840</v>
       </c>
-      <c r="AH53" s="3">
+      <c r="AH53" s="4">
         <f>F53*AE53*DATOS!$D$6+'COST PER TASK'!G53*'COST PER TASK'!AE53*DATOS!$D$7+'COST PER TASK'!H53*'COST PER TASK'!AE53*DATOS!$D$8+'COST PER TASK'!I53*'COST PER TASK'!AE53*DATOS!$D$9+'COST PER TASK'!J53*'COST PER TASK'!AE53*DATOS!$D$10+'COST PER TASK'!K53*'COST PER TASK'!AE53*DATOS!$D$11+'COST PER TASK'!L53*'COST PER TASK'!AE53*DATOS!$D$12+'COST PER TASK'!M53*'COST PER TASK'!AE53*DATOS!$D$13+'COST PER TASK'!N53*'COST PER TASK'!AE53*DATOS!$D$14+'COST PER TASK'!O53*'COST PER TASK'!AE53*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI53" s="3">
+      <c r="AI53" s="4">
         <f>'COST PER TASK'!P53*'COST PER TASK'!AE53*DATOS!$D$16+'COST PER TASK'!Q53*'COST PER TASK'!AE53*DATOS!$D$17+'COST PER TASK'!R53*'COST PER TASK'!AE53*DATOS!$D$18+'COST PER TASK'!S53*'COST PER TASK'!AE53*DATOS!$D$19+'COST PER TASK'!T53*'COST PER TASK'!AE53*DATOS!$D$20+'COST PER TASK'!U53*'COST PER TASK'!AE53*DATOS!$D$21+'COST PER TASK'!V53*'COST PER TASK'!AE53*DATOS!$D$22</f>
         <v>77648.496240601511</v>
       </c>
+      <c r="AJ53" s="4">
+        <f>'COST PER TASK'!W53*'COST PER TASK'!AE53*DATOS!$B$23+'COST PER TASK'!X53*'COST PER TASK'!AE53*DATOS!$B$24+'COST PER TASK'!Y53*'COST PER TASK'!AE53*DATOS!$B$25+'COST PER TASK'!Z53*'COST PER TASK'!AE53*DATOS!$B$26+'COST PER TASK'!AA53*'COST PER TASK'!AE53*DATOS!$B$27+'COST PER TASK'!AB53*'COST PER TASK'!AE53*DATOS!$B$28+'COST PER TASK'!AC53*'COST PER TASK'!AE53*DATOS!$B$29</f>
+        <v>5760</v>
+      </c>
       <c r="AK53" s="8">
         <f t="shared" si="1"/>
-        <v>87488.496240601511</v>
+        <v>93248.496240601511</v>
       </c>
       <c r="AL53" s="8">
         <f t="shared" si="2"/>
-        <v>1458.1416040100253</v>
+        <v>1554.1416040100253</v>
       </c>
     </row>
     <row r="54" spans="2:38" x14ac:dyDescent="0.2">
@@ -4460,21 +4665,25 @@
         <f>AF54*C54*DATOS!$B$3+'COST PER TASK'!AF54*'COST PER TASK'!D54*DATOS!$B$4+'COST PER TASK'!AF54*'COST PER TASK'!E54*DATOS!$B$5</f>
         <v>1168</v>
       </c>
-      <c r="AH54" s="3">
+      <c r="AH54" s="4">
         <f>F54*AE54*DATOS!$D$6+'COST PER TASK'!G54*'COST PER TASK'!AE54*DATOS!$D$7+'COST PER TASK'!H54*'COST PER TASK'!AE54*DATOS!$D$8+'COST PER TASK'!I54*'COST PER TASK'!AE54*DATOS!$D$9+'COST PER TASK'!J54*'COST PER TASK'!AE54*DATOS!$D$10+'COST PER TASK'!K54*'COST PER TASK'!AE54*DATOS!$D$11+'COST PER TASK'!L54*'COST PER TASK'!AE54*DATOS!$D$12+'COST PER TASK'!M54*'COST PER TASK'!AE54*DATOS!$D$13+'COST PER TASK'!N54*'COST PER TASK'!AE54*DATOS!$D$14+'COST PER TASK'!O54*'COST PER TASK'!AE54*DATOS!$D$15</f>
         <v>28.311955302670384</v>
       </c>
-      <c r="AI54" s="3">
+      <c r="AI54" s="4">
         <f>'COST PER TASK'!P54*'COST PER TASK'!AE54*DATOS!$D$16+'COST PER TASK'!Q54*'COST PER TASK'!AE54*DATOS!$D$17+'COST PER TASK'!R54*'COST PER TASK'!AE54*DATOS!$D$18+'COST PER TASK'!S54*'COST PER TASK'!AE54*DATOS!$D$19+'COST PER TASK'!T54*'COST PER TASK'!AE54*DATOS!$D$20+'COST PER TASK'!U54*'COST PER TASK'!AE54*DATOS!$D$21+'COST PER TASK'!V54*'COST PER TASK'!AE54*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ54" s="4">
+        <f>'COST PER TASK'!W54*'COST PER TASK'!AE54*DATOS!$B$23+'COST PER TASK'!X54*'COST PER TASK'!AE54*DATOS!$B$24+'COST PER TASK'!Y54*'COST PER TASK'!AE54*DATOS!$B$25+'COST PER TASK'!Z54*'COST PER TASK'!AE54*DATOS!$B$26+'COST PER TASK'!AA54*'COST PER TASK'!AE54*DATOS!$B$27+'COST PER TASK'!AB54*'COST PER TASK'!AE54*DATOS!$B$28+'COST PER TASK'!AC54*'COST PER TASK'!AE54*DATOS!$B$29</f>
+        <v>320</v>
+      </c>
       <c r="AK54" s="8">
         <f t="shared" si="1"/>
-        <v>1196.3119553026704</v>
+        <v>1516.3119553026704</v>
       </c>
       <c r="AL54" s="8">
         <f t="shared" si="2"/>
-        <v>149.5389944128338</v>
+        <v>189.5389944128338</v>
       </c>
     </row>
     <row r="55" spans="2:38" x14ac:dyDescent="0.2">
@@ -4511,21 +4720,25 @@
         <f>AF55*C55*DATOS!$B$3+'COST PER TASK'!AF55*'COST PER TASK'!D55*DATOS!$B$4+'COST PER TASK'!AF55*'COST PER TASK'!E55*DATOS!$B$5</f>
         <v>730</v>
       </c>
-      <c r="AH55" s="3">
+      <c r="AH55" s="4">
         <f>F55*AE55*DATOS!$D$6+'COST PER TASK'!G55*'COST PER TASK'!AE55*DATOS!$D$7+'COST PER TASK'!H55*'COST PER TASK'!AE55*DATOS!$D$8+'COST PER TASK'!I55*'COST PER TASK'!AE55*DATOS!$D$9+'COST PER TASK'!J55*'COST PER TASK'!AE55*DATOS!$D$10+'COST PER TASK'!K55*'COST PER TASK'!AE55*DATOS!$D$11+'COST PER TASK'!L55*'COST PER TASK'!AE55*DATOS!$D$12+'COST PER TASK'!M55*'COST PER TASK'!AE55*DATOS!$D$13+'COST PER TASK'!N55*'COST PER TASK'!AE55*DATOS!$D$14+'COST PER TASK'!O55*'COST PER TASK'!AE55*DATOS!$D$15</f>
         <v>17.69497206416899</v>
       </c>
-      <c r="AI55" s="3">
+      <c r="AI55" s="4">
         <f>'COST PER TASK'!P55*'COST PER TASK'!AE55*DATOS!$D$16+'COST PER TASK'!Q55*'COST PER TASK'!AE55*DATOS!$D$17+'COST PER TASK'!R55*'COST PER TASK'!AE55*DATOS!$D$18+'COST PER TASK'!S55*'COST PER TASK'!AE55*DATOS!$D$19+'COST PER TASK'!T55*'COST PER TASK'!AE55*DATOS!$D$20+'COST PER TASK'!U55*'COST PER TASK'!AE55*DATOS!$D$21+'COST PER TASK'!V55*'COST PER TASK'!AE55*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ55" s="4">
+        <f>'COST PER TASK'!W55*'COST PER TASK'!AE55*DATOS!$B$23+'COST PER TASK'!X55*'COST PER TASK'!AE55*DATOS!$B$24+'COST PER TASK'!Y55*'COST PER TASK'!AE55*DATOS!$B$25+'COST PER TASK'!Z55*'COST PER TASK'!AE55*DATOS!$B$26+'COST PER TASK'!AA55*'COST PER TASK'!AE55*DATOS!$B$27+'COST PER TASK'!AB55*'COST PER TASK'!AE55*DATOS!$B$28+'COST PER TASK'!AC55*'COST PER TASK'!AE55*DATOS!$B$29</f>
+        <v>200</v>
+      </c>
       <c r="AK55" s="8">
         <f t="shared" si="1"/>
-        <v>747.69497206416895</v>
+        <v>947.69497206416895</v>
       </c>
       <c r="AL55" s="8">
         <f t="shared" si="2"/>
-        <v>149.5389944128338</v>
+        <v>189.5389944128338</v>
       </c>
     </row>
     <row r="56" spans="2:38" x14ac:dyDescent="0.2">
@@ -4562,21 +4775,25 @@
         <f>AF56*C56*DATOS!$B$3+'COST PER TASK'!AF56*'COST PER TASK'!D56*DATOS!$B$4+'COST PER TASK'!AF56*'COST PER TASK'!E56*DATOS!$B$5</f>
         <v>1520</v>
       </c>
-      <c r="AH56" s="3">
+      <c r="AH56" s="4">
         <f>F56*AE56*DATOS!$D$6+'COST PER TASK'!G56*'COST PER TASK'!AE56*DATOS!$D$7+'COST PER TASK'!H56*'COST PER TASK'!AE56*DATOS!$D$8+'COST PER TASK'!I56*'COST PER TASK'!AE56*DATOS!$D$9+'COST PER TASK'!J56*'COST PER TASK'!AE56*DATOS!$D$10+'COST PER TASK'!K56*'COST PER TASK'!AE56*DATOS!$D$11+'COST PER TASK'!L56*'COST PER TASK'!AE56*DATOS!$D$12+'COST PER TASK'!M56*'COST PER TASK'!AE56*DATOS!$D$13+'COST PER TASK'!N56*'COST PER TASK'!AE56*DATOS!$D$14+'COST PER TASK'!O56*'COST PER TASK'!AE56*DATOS!$D$15</f>
         <v>35.38994412833798</v>
       </c>
-      <c r="AI56" s="3">
+      <c r="AI56" s="4">
         <f>'COST PER TASK'!P56*'COST PER TASK'!AE56*DATOS!$D$16+'COST PER TASK'!Q56*'COST PER TASK'!AE56*DATOS!$D$17+'COST PER TASK'!R56*'COST PER TASK'!AE56*DATOS!$D$18+'COST PER TASK'!S56*'COST PER TASK'!AE56*DATOS!$D$19+'COST PER TASK'!T56*'COST PER TASK'!AE56*DATOS!$D$20+'COST PER TASK'!U56*'COST PER TASK'!AE56*DATOS!$D$21+'COST PER TASK'!V56*'COST PER TASK'!AE56*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ56" s="4">
+        <f>'COST PER TASK'!W56*'COST PER TASK'!AE56*DATOS!$B$23+'COST PER TASK'!X56*'COST PER TASK'!AE56*DATOS!$B$24+'COST PER TASK'!Y56*'COST PER TASK'!AE56*DATOS!$B$25+'COST PER TASK'!Z56*'COST PER TASK'!AE56*DATOS!$B$26+'COST PER TASK'!AA56*'COST PER TASK'!AE56*DATOS!$B$27+'COST PER TASK'!AB56*'COST PER TASK'!AE56*DATOS!$B$28+'COST PER TASK'!AC56*'COST PER TASK'!AE56*DATOS!$B$29</f>
+        <v>400</v>
+      </c>
       <c r="AK56" s="8">
         <f t="shared" si="1"/>
-        <v>1555.3899441283379</v>
+        <v>1955.3899441283379</v>
       </c>
       <c r="AL56" s="8">
         <f t="shared" si="2"/>
-        <v>155.5389944128338</v>
+        <v>195.5389944128338</v>
       </c>
     </row>
     <row r="57" spans="2:38" x14ac:dyDescent="0.2">
@@ -4616,21 +4833,25 @@
         <f>AF57*C57*DATOS!$B$3+'COST PER TASK'!AF57*'COST PER TASK'!D57*DATOS!$B$4+'COST PER TASK'!AF57*'COST PER TASK'!E57*DATOS!$B$5</f>
         <v>1254.4000000000001</v>
       </c>
-      <c r="AH57" s="3">
+      <c r="AH57" s="4">
         <f>F57*AE57*DATOS!$D$6+'COST PER TASK'!G57*'COST PER TASK'!AE57*DATOS!$D$7+'COST PER TASK'!H57*'COST PER TASK'!AE57*DATOS!$D$8+'COST PER TASK'!I57*'COST PER TASK'!AE57*DATOS!$D$9+'COST PER TASK'!J57*'COST PER TASK'!AE57*DATOS!$D$10+'COST PER TASK'!K57*'COST PER TASK'!AE57*DATOS!$D$11+'COST PER TASK'!L57*'COST PER TASK'!AE57*DATOS!$D$12+'COST PER TASK'!M57*'COST PER TASK'!AE57*DATOS!$D$13+'COST PER TASK'!N57*'COST PER TASK'!AE57*DATOS!$D$14+'COST PER TASK'!O57*'COST PER TASK'!AE57*DATOS!$D$15</f>
         <v>192.31195530267038</v>
       </c>
-      <c r="AI57" s="3">
+      <c r="AI57" s="4">
         <f>'COST PER TASK'!P57*'COST PER TASK'!AE57*DATOS!$D$16+'COST PER TASK'!Q57*'COST PER TASK'!AE57*DATOS!$D$17+'COST PER TASK'!R57*'COST PER TASK'!AE57*DATOS!$D$18+'COST PER TASK'!S57*'COST PER TASK'!AE57*DATOS!$D$19+'COST PER TASK'!T57*'COST PER TASK'!AE57*DATOS!$D$20+'COST PER TASK'!U57*'COST PER TASK'!AE57*DATOS!$D$21+'COST PER TASK'!V57*'COST PER TASK'!AE57*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ57" s="4">
+        <f>'COST PER TASK'!W57*'COST PER TASK'!AE57*DATOS!$B$23+'COST PER TASK'!X57*'COST PER TASK'!AE57*DATOS!$B$24+'COST PER TASK'!Y57*'COST PER TASK'!AE57*DATOS!$B$25+'COST PER TASK'!Z57*'COST PER TASK'!AE57*DATOS!$B$26+'COST PER TASK'!AA57*'COST PER TASK'!AE57*DATOS!$B$27+'COST PER TASK'!AB57*'COST PER TASK'!AE57*DATOS!$B$28+'COST PER TASK'!AC57*'COST PER TASK'!AE57*DATOS!$B$29</f>
+        <v>320</v>
+      </c>
       <c r="AK57" s="8">
         <f t="shared" si="1"/>
-        <v>1446.7119553026705</v>
+        <v>1766.7119553026705</v>
       </c>
       <c r="AL57" s="8">
         <f t="shared" si="2"/>
-        <v>180.83899441283381</v>
+        <v>220.83899441283381</v>
       </c>
     </row>
     <row r="58" spans="2:38" x14ac:dyDescent="0.2">
@@ -4670,21 +4891,25 @@
         <f>AF58*C58*DATOS!$B$3+'COST PER TASK'!AF58*'COST PER TASK'!D58*DATOS!$B$4+'COST PER TASK'!AF58*'COST PER TASK'!E58*DATOS!$B$5</f>
         <v>3800</v>
       </c>
-      <c r="AH58" s="3">
+      <c r="AH58" s="4">
         <f>F58*AE58*DATOS!$D$6+'COST PER TASK'!G58*'COST PER TASK'!AE58*DATOS!$D$7+'COST PER TASK'!H58*'COST PER TASK'!AE58*DATOS!$D$8+'COST PER TASK'!I58*'COST PER TASK'!AE58*DATOS!$D$9+'COST PER TASK'!J58*'COST PER TASK'!AE58*DATOS!$D$10+'COST PER TASK'!K58*'COST PER TASK'!AE58*DATOS!$D$11+'COST PER TASK'!L58*'COST PER TASK'!AE58*DATOS!$D$12+'COST PER TASK'!M58*'COST PER TASK'!AE58*DATOS!$D$13+'COST PER TASK'!N58*'COST PER TASK'!AE58*DATOS!$D$14+'COST PER TASK'!O58*'COST PER TASK'!AE58*DATOS!$D$15</f>
         <v>88.474860320844954</v>
       </c>
-      <c r="AI58" s="3">
+      <c r="AI58" s="4">
         <f>'COST PER TASK'!P58*'COST PER TASK'!AE58*DATOS!$D$16+'COST PER TASK'!Q58*'COST PER TASK'!AE58*DATOS!$D$17+'COST PER TASK'!R58*'COST PER TASK'!AE58*DATOS!$D$18+'COST PER TASK'!S58*'COST PER TASK'!AE58*DATOS!$D$19+'COST PER TASK'!T58*'COST PER TASK'!AE58*DATOS!$D$20+'COST PER TASK'!U58*'COST PER TASK'!AE58*DATOS!$D$21+'COST PER TASK'!V58*'COST PER TASK'!AE58*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ58" s="4">
+        <f>'COST PER TASK'!W58*'COST PER TASK'!AE58*DATOS!$B$23+'COST PER TASK'!X58*'COST PER TASK'!AE58*DATOS!$B$24+'COST PER TASK'!Y58*'COST PER TASK'!AE58*DATOS!$B$25+'COST PER TASK'!Z58*'COST PER TASK'!AE58*DATOS!$B$26+'COST PER TASK'!AA58*'COST PER TASK'!AE58*DATOS!$B$27+'COST PER TASK'!AB58*'COST PER TASK'!AE58*DATOS!$B$28+'COST PER TASK'!AC58*'COST PER TASK'!AE58*DATOS!$B$29</f>
+        <v>1000</v>
+      </c>
       <c r="AK58" s="8">
         <f t="shared" si="1"/>
-        <v>3888.474860320845</v>
+        <v>4888.4748603208445</v>
       </c>
       <c r="AL58" s="8">
         <f t="shared" si="2"/>
-        <v>155.5389944128338</v>
+        <v>195.53899441283377</v>
       </c>
     </row>
     <row r="59" spans="2:38" x14ac:dyDescent="0.2">
@@ -4718,21 +4943,25 @@
         <f>AF59*C59*DATOS!$B$3+'COST PER TASK'!AF59*'COST PER TASK'!D59*DATOS!$B$4+'COST PER TASK'!AF59*'COST PER TASK'!E59*DATOS!$B$5</f>
         <v>13680</v>
       </c>
-      <c r="AH59" s="3">
+      <c r="AH59" s="4">
         <f>F59*AE59*DATOS!$D$6+'COST PER TASK'!G59*'COST PER TASK'!AE59*DATOS!$D$7+'COST PER TASK'!H59*'COST PER TASK'!AE59*DATOS!$D$8+'COST PER TASK'!I59*'COST PER TASK'!AE59*DATOS!$D$9+'COST PER TASK'!J59*'COST PER TASK'!AE59*DATOS!$D$10+'COST PER TASK'!K59*'COST PER TASK'!AE59*DATOS!$D$11+'COST PER TASK'!L59*'COST PER TASK'!AE59*DATOS!$D$12+'COST PER TASK'!M59*'COST PER TASK'!AE59*DATOS!$D$13+'COST PER TASK'!N59*'COST PER TASK'!AE59*DATOS!$D$14+'COST PER TASK'!O59*'COST PER TASK'!AE59*DATOS!$D$15</f>
         <v>676.5</v>
       </c>
-      <c r="AI59" s="3">
+      <c r="AI59" s="4">
         <f>'COST PER TASK'!P59*'COST PER TASK'!AE59*DATOS!$D$16+'COST PER TASK'!Q59*'COST PER TASK'!AE59*DATOS!$D$17+'COST PER TASK'!R59*'COST PER TASK'!AE59*DATOS!$D$18+'COST PER TASK'!S59*'COST PER TASK'!AE59*DATOS!$D$19+'COST PER TASK'!T59*'COST PER TASK'!AE59*DATOS!$D$20+'COST PER TASK'!U59*'COST PER TASK'!AE59*DATOS!$D$21+'COST PER TASK'!V59*'COST PER TASK'!AE59*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ59" s="4">
+        <f>'COST PER TASK'!W59*'COST PER TASK'!AE59*DATOS!$B$23+'COST PER TASK'!X59*'COST PER TASK'!AE59*DATOS!$B$24+'COST PER TASK'!Y59*'COST PER TASK'!AE59*DATOS!$B$25+'COST PER TASK'!Z59*'COST PER TASK'!AE59*DATOS!$B$26+'COST PER TASK'!AA59*'COST PER TASK'!AE59*DATOS!$B$27+'COST PER TASK'!AB59*'COST PER TASK'!AE59*DATOS!$B$28+'COST PER TASK'!AC59*'COST PER TASK'!AE59*DATOS!$B$29</f>
+        <v>3600</v>
+      </c>
       <c r="AK59" s="8">
         <f t="shared" si="1"/>
-        <v>14356.5</v>
+        <v>17956.5</v>
       </c>
       <c r="AL59" s="8">
         <f t="shared" si="2"/>
-        <v>159.51666666666668</v>
+        <v>199.51666666666668</v>
       </c>
     </row>
     <row r="60" spans="2:38" x14ac:dyDescent="0.2">
@@ -4763,21 +4992,25 @@
         <f>AF60*C60*DATOS!$B$3+'COST PER TASK'!AF60*'COST PER TASK'!D60*DATOS!$B$4+'COST PER TASK'!AF60*'COST PER TASK'!E60*DATOS!$B$5</f>
         <v>117040</v>
       </c>
-      <c r="AH60" s="3">
+      <c r="AH60" s="4">
         <f>F60*AE60*DATOS!$D$6+'COST PER TASK'!G60*'COST PER TASK'!AE60*DATOS!$D$7+'COST PER TASK'!H60*'COST PER TASK'!AE60*DATOS!$D$8+'COST PER TASK'!I60*'COST PER TASK'!AE60*DATOS!$D$9+'COST PER TASK'!J60*'COST PER TASK'!AE60*DATOS!$D$10+'COST PER TASK'!K60*'COST PER TASK'!AE60*DATOS!$D$11+'COST PER TASK'!L60*'COST PER TASK'!AE60*DATOS!$D$12+'COST PER TASK'!M60*'COST PER TASK'!AE60*DATOS!$D$13+'COST PER TASK'!N60*'COST PER TASK'!AE60*DATOS!$D$14+'COST PER TASK'!O60*'COST PER TASK'!AE60*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI60" s="3">
+      <c r="AI60" s="4">
         <f>'COST PER TASK'!P60*'COST PER TASK'!AE60*DATOS!$D$16+'COST PER TASK'!Q60*'COST PER TASK'!AE60*DATOS!$D$17+'COST PER TASK'!R60*'COST PER TASK'!AE60*DATOS!$D$18+'COST PER TASK'!S60*'COST PER TASK'!AE60*DATOS!$D$19+'COST PER TASK'!T60*'COST PER TASK'!AE60*DATOS!$D$20+'COST PER TASK'!U60*'COST PER TASK'!AE60*DATOS!$D$21+'COST PER TASK'!V60*'COST PER TASK'!AE60*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ60" s="4">
+        <f>'COST PER TASK'!W60*'COST PER TASK'!AE60*DATOS!$B$23+'COST PER TASK'!X60*'COST PER TASK'!AE60*DATOS!$B$24+'COST PER TASK'!Y60*'COST PER TASK'!AE60*DATOS!$B$25+'COST PER TASK'!Z60*'COST PER TASK'!AE60*DATOS!$B$26+'COST PER TASK'!AA60*'COST PER TASK'!AE60*DATOS!$B$27+'COST PER TASK'!AB60*'COST PER TASK'!AE60*DATOS!$B$28+'COST PER TASK'!AC60*'COST PER TASK'!AE60*DATOS!$B$29</f>
+        <v>30800</v>
+      </c>
       <c r="AK60" s="8">
         <f t="shared" si="1"/>
-        <v>117040</v>
+        <v>147840</v>
       </c>
       <c r="AL60" s="8">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="2:38" x14ac:dyDescent="0.2">
@@ -4811,21 +5044,25 @@
         <f>AF61*C61*DATOS!$B$3+'COST PER TASK'!AF61*'COST PER TASK'!D61*DATOS!$B$4+'COST PER TASK'!AF61*'COST PER TASK'!E61*DATOS!$B$5</f>
         <v>130720</v>
       </c>
-      <c r="AH61" s="3">
+      <c r="AH61" s="4">
         <f>F61*AE61*DATOS!$D$6+'COST PER TASK'!G61*'COST PER TASK'!AE61*DATOS!$D$7+'COST PER TASK'!H61*'COST PER TASK'!AE61*DATOS!$D$8+'COST PER TASK'!I61*'COST PER TASK'!AE61*DATOS!$D$9+'COST PER TASK'!J61*'COST PER TASK'!AE61*DATOS!$D$10+'COST PER TASK'!K61*'COST PER TASK'!AE61*DATOS!$D$11+'COST PER TASK'!L61*'COST PER TASK'!AE61*DATOS!$D$12+'COST PER TASK'!M61*'COST PER TASK'!AE61*DATOS!$D$13+'COST PER TASK'!N61*'COST PER TASK'!AE61*DATOS!$D$14+'COST PER TASK'!O61*'COST PER TASK'!AE61*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI61" s="3">
+      <c r="AI61" s="4">
         <f>'COST PER TASK'!P61*'COST PER TASK'!AE61*DATOS!$D$16+'COST PER TASK'!Q61*'COST PER TASK'!AE61*DATOS!$D$17+'COST PER TASK'!R61*'COST PER TASK'!AE61*DATOS!$D$18+'COST PER TASK'!S61*'COST PER TASK'!AE61*DATOS!$D$19+'COST PER TASK'!T61*'COST PER TASK'!AE61*DATOS!$D$20+'COST PER TASK'!U61*'COST PER TASK'!AE61*DATOS!$D$21+'COST PER TASK'!V61*'COST PER TASK'!AE61*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ61" s="4">
+        <f>'COST PER TASK'!W61*'COST PER TASK'!AE61*DATOS!$B$23+'COST PER TASK'!X61*'COST PER TASK'!AE61*DATOS!$B$24+'COST PER TASK'!Y61*'COST PER TASK'!AE61*DATOS!$B$25+'COST PER TASK'!Z61*'COST PER TASK'!AE61*DATOS!$B$26+'COST PER TASK'!AA61*'COST PER TASK'!AE61*DATOS!$B$27+'COST PER TASK'!AB61*'COST PER TASK'!AE61*DATOS!$B$28+'COST PER TASK'!AC61*'COST PER TASK'!AE61*DATOS!$B$29</f>
+        <v>13760</v>
+      </c>
       <c r="AK61" s="8">
         <f t="shared" si="1"/>
-        <v>130720</v>
+        <v>144480</v>
       </c>
       <c r="AL61" s="8">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="2:38" x14ac:dyDescent="0.2">
@@ -4856,21 +5093,25 @@
         <f>AF62*C62*DATOS!$B$3+'COST PER TASK'!AF62*'COST PER TASK'!D62*DATOS!$B$4+'COST PER TASK'!AF62*'COST PER TASK'!E62*DATOS!$B$5</f>
         <v>130720</v>
       </c>
-      <c r="AH62" s="3">
+      <c r="AH62" s="4">
         <f>F62*AE62*DATOS!$D$6+'COST PER TASK'!G62*'COST PER TASK'!AE62*DATOS!$D$7+'COST PER TASK'!H62*'COST PER TASK'!AE62*DATOS!$D$8+'COST PER TASK'!I62*'COST PER TASK'!AE62*DATOS!$D$9+'COST PER TASK'!J62*'COST PER TASK'!AE62*DATOS!$D$10+'COST PER TASK'!K62*'COST PER TASK'!AE62*DATOS!$D$11+'COST PER TASK'!L62*'COST PER TASK'!AE62*DATOS!$D$12+'COST PER TASK'!M62*'COST PER TASK'!AE62*DATOS!$D$13+'COST PER TASK'!N62*'COST PER TASK'!AE62*DATOS!$D$14+'COST PER TASK'!O62*'COST PER TASK'!AE62*DATOS!$D$15</f>
         <v>0</v>
       </c>
-      <c r="AI62" s="3">
+      <c r="AI62" s="4">
         <f>'COST PER TASK'!P62*'COST PER TASK'!AE62*DATOS!$D$16+'COST PER TASK'!Q62*'COST PER TASK'!AE62*DATOS!$D$17+'COST PER TASK'!R62*'COST PER TASK'!AE62*DATOS!$D$18+'COST PER TASK'!S62*'COST PER TASK'!AE62*DATOS!$D$19+'COST PER TASK'!T62*'COST PER TASK'!AE62*DATOS!$D$20+'COST PER TASK'!U62*'COST PER TASK'!AE62*DATOS!$D$21+'COST PER TASK'!V62*'COST PER TASK'!AE62*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ62" s="4">
+        <f>'COST PER TASK'!W62*'COST PER TASK'!AE62*DATOS!$B$23+'COST PER TASK'!X62*'COST PER TASK'!AE62*DATOS!$B$24+'COST PER TASK'!Y62*'COST PER TASK'!AE62*DATOS!$B$25+'COST PER TASK'!Z62*'COST PER TASK'!AE62*DATOS!$B$26+'COST PER TASK'!AA62*'COST PER TASK'!AE62*DATOS!$B$27+'COST PER TASK'!AB62*'COST PER TASK'!AE62*DATOS!$B$28+'COST PER TASK'!AC62*'COST PER TASK'!AE62*DATOS!$B$29</f>
+        <v>6880</v>
+      </c>
       <c r="AK62" s="8">
         <f t="shared" si="1"/>
-        <v>130720</v>
+        <v>137600</v>
       </c>
       <c r="AL62" s="8">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="2:38" x14ac:dyDescent="0.2">
@@ -4907,21 +5148,25 @@
         <f>AF63*C63*DATOS!$B$3+'COST PER TASK'!AF63*'COST PER TASK'!D63*DATOS!$B$4+'COST PER TASK'!AF63*'COST PER TASK'!E63*DATOS!$B$5</f>
         <v>130720</v>
       </c>
-      <c r="AH63" s="3">
+      <c r="AH63" s="4">
         <f>F63*AE63*DATOS!$D$6+'COST PER TASK'!G63*'COST PER TASK'!AE63*DATOS!$D$7+'COST PER TASK'!H63*'COST PER TASK'!AE63*DATOS!$D$8+'COST PER TASK'!I63*'COST PER TASK'!AE63*DATOS!$D$9+'COST PER TASK'!J63*'COST PER TASK'!AE63*DATOS!$D$10+'COST PER TASK'!K63*'COST PER TASK'!AE63*DATOS!$D$11+'COST PER TASK'!L63*'COST PER TASK'!AE63*DATOS!$D$12+'COST PER TASK'!M63*'COST PER TASK'!AE63*DATOS!$D$13+'COST PER TASK'!N63*'COST PER TASK'!AE63*DATOS!$D$14+'COST PER TASK'!O63*'COST PER TASK'!AE63*DATOS!$D$15</f>
         <v>738.0635771734967</v>
       </c>
-      <c r="AI63" s="3">
+      <c r="AI63" s="4">
         <f>'COST PER TASK'!P63*'COST PER TASK'!AE63*DATOS!$D$16+'COST PER TASK'!Q63*'COST PER TASK'!AE63*DATOS!$D$17+'COST PER TASK'!R63*'COST PER TASK'!AE63*DATOS!$D$18+'COST PER TASK'!S63*'COST PER TASK'!AE63*DATOS!$D$19+'COST PER TASK'!T63*'COST PER TASK'!AE63*DATOS!$D$20+'COST PER TASK'!U63*'COST PER TASK'!AE63*DATOS!$D$21+'COST PER TASK'!V63*'COST PER TASK'!AE63*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ63" s="4">
+        <f>'COST PER TASK'!W63*'COST PER TASK'!AE63*DATOS!$B$23+'COST PER TASK'!X63*'COST PER TASK'!AE63*DATOS!$B$24+'COST PER TASK'!Y63*'COST PER TASK'!AE63*DATOS!$B$25+'COST PER TASK'!Z63*'COST PER TASK'!AE63*DATOS!$B$26+'COST PER TASK'!AA63*'COST PER TASK'!AE63*DATOS!$B$27+'COST PER TASK'!AB63*'COST PER TASK'!AE63*DATOS!$B$28+'COST PER TASK'!AC63*'COST PER TASK'!AE63*DATOS!$B$29</f>
+        <v>68800</v>
+      </c>
       <c r="AK63" s="8">
         <f t="shared" si="1"/>
-        <v>131458.06357717351</v>
+        <v>200258.06357717351</v>
       </c>
       <c r="AL63" s="8">
         <f t="shared" si="2"/>
-        <v>152.85821346182965</v>
+        <v>232.85821346182965</v>
       </c>
     </row>
     <row r="64" spans="2:38" x14ac:dyDescent="0.2">
@@ -4958,21 +5203,25 @@
         <f>AF64*C64*DATOS!$B$3+'COST PER TASK'!AF64*'COST PER TASK'!D64*DATOS!$B$4+'COST PER TASK'!AF64*'COST PER TASK'!E64*DATOS!$B$5</f>
         <v>130720</v>
       </c>
-      <c r="AH64" s="3">
+      <c r="AH64" s="4">
         <f>F64*AE64*DATOS!$D$6+'COST PER TASK'!G64*'COST PER TASK'!AE64*DATOS!$D$7+'COST PER TASK'!H64*'COST PER TASK'!AE64*DATOS!$D$8+'COST PER TASK'!I64*'COST PER TASK'!AE64*DATOS!$D$9+'COST PER TASK'!J64*'COST PER TASK'!AE64*DATOS!$D$10+'COST PER TASK'!K64*'COST PER TASK'!AE64*DATOS!$D$11+'COST PER TASK'!L64*'COST PER TASK'!AE64*DATOS!$D$12+'COST PER TASK'!M64*'COST PER TASK'!AE64*DATOS!$D$13+'COST PER TASK'!N64*'COST PER TASK'!AE64*DATOS!$D$14+'COST PER TASK'!O64*'COST PER TASK'!AE64*DATOS!$D$15</f>
         <v>738.0635771734967</v>
       </c>
-      <c r="AI64" s="3">
+      <c r="AI64" s="4">
         <f>'COST PER TASK'!P64*'COST PER TASK'!AE64*DATOS!$D$16+'COST PER TASK'!Q64*'COST PER TASK'!AE64*DATOS!$D$17+'COST PER TASK'!R64*'COST PER TASK'!AE64*DATOS!$D$18+'COST PER TASK'!S64*'COST PER TASK'!AE64*DATOS!$D$19+'COST PER TASK'!T64*'COST PER TASK'!AE64*DATOS!$D$20+'COST PER TASK'!U64*'COST PER TASK'!AE64*DATOS!$D$21+'COST PER TASK'!V64*'COST PER TASK'!AE64*DATOS!$D$22</f>
         <v>0</v>
       </c>
+      <c r="AJ64" s="4">
+        <f>'COST PER TASK'!W64*'COST PER TASK'!AE64*DATOS!$B$23+'COST PER TASK'!X64*'COST PER TASK'!AE64*DATOS!$B$24+'COST PER TASK'!Y64*'COST PER TASK'!AE64*DATOS!$B$25+'COST PER TASK'!Z64*'COST PER TASK'!AE64*DATOS!$B$26+'COST PER TASK'!AA64*'COST PER TASK'!AE64*DATOS!$B$27+'COST PER TASK'!AB64*'COST PER TASK'!AE64*DATOS!$B$28+'COST PER TASK'!AC64*'COST PER TASK'!AE64*DATOS!$B$29</f>
+        <v>34400</v>
+      </c>
       <c r="AK64" s="8">
         <f t="shared" si="1"/>
-        <v>131458.06357717351</v>
+        <v>165858.06357717351</v>
       </c>
       <c r="AL64" s="8">
         <f t="shared" si="2"/>
-        <v>152.85821346182965</v>
+        <v>192.85821346182965</v>
       </c>
     </row>
     <row r="65" spans="6:37" x14ac:dyDescent="0.2">
@@ -5076,17 +5325,21 @@
         <f>SUM(AG2:AG64)</f>
         <v>2414381.5428571426</v>
       </c>
-      <c r="AH65" s="18">
+      <c r="AH65" s="17">
         <f>SUM(AH2:AH64)</f>
         <v>42064.5</v>
       </c>
-      <c r="AI65" s="18">
+      <c r="AI65" s="17">
         <f>SUM(AI2:AI64)</f>
         <v>460000.00000000006</v>
       </c>
-      <c r="AK65" s="19">
+      <c r="AJ65" s="17">
+        <f>SUM(AJ2:AJ64)</f>
+        <v>712440</v>
+      </c>
+      <c r="AK65" s="18">
         <f>SUM(AK2:AK64)</f>
-        <v>2916446.0428571422</v>
+        <v>3628886.0428571422</v>
       </c>
     </row>
   </sheetData>
@@ -11592,8 +11845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>